<commit_message>
Add RX8900 IIC read write
</commit_message>
<xml_diff>
--- a/Software/MDK-ARM/Software_analysis.xlsx
+++ b/Software/MDK-ARM/Software_analysis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
   <si>
     <t>Software</t>
   </si>
@@ -41,6 +41,9 @@
     <t>libspace.o</t>
   </si>
   <si>
+    <t>i2c.o</t>
+  </si>
+  <si>
     <t>tx_initialize_high_level.o</t>
   </si>
   <si>
@@ -56,6 +59,15 @@
     <t>stm32l4xx_hal_rcc.o</t>
   </si>
   <si>
+    <t>stm32l4xx_hal_i2c.o</t>
+  </si>
+  <si>
+    <t>stm32l4xx_hal_rcc_ex.o</t>
+  </si>
+  <si>
+    <t>stm32l4xx_hal_gpio.o</t>
+  </si>
+  <si>
     <t>txe_thread_create.o</t>
   </si>
   <si>
@@ -89,15 +101,18 @@
     <t>tx_initialize_low_level.o</t>
   </si>
   <si>
+    <t>main.o</t>
+  </si>
+  <si>
     <t>tx_thread_sleep.o</t>
   </si>
   <si>
+    <t>stm32l4xx_hal_i2c_ex.o</t>
+  </si>
+  <si>
     <t>tx_byte_pool_create.o</t>
   </si>
   <si>
-    <t>main.o</t>
-  </si>
-  <si>
     <t>tx_thread_time_slice.o</t>
   </si>
   <si>
@@ -108,6 +123,12 @@
   </si>
   <si>
     <t>tx_thread_shell_entry.o</t>
+  </si>
+  <si>
+    <t>rx8900_callout.o</t>
+  </si>
+  <si>
+    <t>rx8900.o</t>
   </si>
   <si>
     <t>rt_memclr_w.o</t>
@@ -320,9 +341,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ram_percent!$A$3:$A$64</c:f>
+              <c:f>ram_percent!$A$3:$A$71</c:f>
               <c:strCache>
-                <c:ptCount val="62"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>startup_stm32l432xx.o</c:v>
                 </c:pt>
@@ -345,18 +366,21 @@
                   <c:v>libspace.o</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>i2c.o</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>tx_initialize_high_level.o</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>stm32l4xx_hal.o</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>tx_low_power.o</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>system_stm32l4xx.o</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="68">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -364,44 +388,47 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ram_percent!$B$3:$B$64</c:f>
+              <c:f>ram_percent!$B$3:$B$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="62"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
-                  <c:v>33.3622932434082</c:v>
+                  <c:v>32.76450347900391</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.06429100036621</c:v>
+                  <c:v>25.59726905822754</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.85317039489746</c:v>
+                  <c:v>18.51535797119141</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.25021743774414</c:v>
+                  <c:v>12.03071689605713</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.735881805419922</c:v>
+                  <c:v>3.668941974639893</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.085143327713013</c:v>
+                  <c:v>2.047781467437744</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.085143327713013</c:v>
+                  <c:v>2.047781467437744</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.129452705383301</c:v>
+                  <c:v>1.791808843612671</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2606429159641266</c:v>
+                  <c:v>1.109215021133423</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.08688097447156906</c:v>
+                  <c:v>0.255972683429718</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.08688097447156906</c:v>
-                </c:pt>
-                <c:pt idx="61">
+                  <c:v>0.0853242352604866</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0853242352604866</c:v>
+                </c:pt>
+                <c:pt idx="68">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -469,193 +496,214 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>flash_percent!$A$3:$A$64</c:f>
+              <c:f>flash_percent!$A$3:$A$71</c:f>
               <c:strCache>
-                <c:ptCount val="62"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>stm32l4xx_hal_rcc.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>stm32l4xx_hal_i2c.o</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>stm32l4xx_hal_rcc_ex.o</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>tx_low_power.o</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>c_w.l</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>startup_stm32l432xx.o</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>stm32l4xx_hal_gpio.o</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>txe_thread_create.o</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>tx_thread_system_suspend.o</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>txe_byte_pool_create.o</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>tx_timer_thread_entry.o</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>tx_thread_create.o</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>tx_thread_system_resume.o</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>stm32l4xx_hal_pwr_ex.o</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
+                  <c:v>i2c.o</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>tx_thread_schedule.o</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="16">
                   <c:v>tx_timer_interrupt.o</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="17">
                   <c:v>stm32l4xx_hal_cortex.o</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="18">
                   <c:v>tx_timer_initialize.o</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="19">
                   <c:v>tx_initialize_low_level.o</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="20">
+                  <c:v>main.o</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>tx_thread_sleep.o</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="22">
+                  <c:v>stm32l4xx_hal_i2c_ex.o</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>tx_byte_pool_create.o</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>main.o</c:v>
-                </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="24">
                   <c:v>stm32l4xx_hal.o</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="25">
                   <c:v>tx_thread_time_slice.o</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="26">
                   <c:v>appmain.o</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="27">
                   <c:v>__scatter.o</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="28">
                   <c:v>tx_timer_system_activate.o</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="29">
                   <c:v>tx_thread_shell_entry.o</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="30">
+                  <c:v>rx8900_callout.o</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>system_stm32l4xx.o</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="32">
+                  <c:v>rx8900.o</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>app_azure_rtos.o</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="34">
                   <c:v>rt_memclr_w.o</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="35">
                   <c:v>tx_initialize_kernel_enter.o</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="36">
                   <c:v>sys_stackheap_outer.o</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="37">
                   <c:v>stm32l4xx_hal_pwr.o</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="38">
                   <c:v>rt_memclr.o</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="39">
                   <c:v>tx_thread_stack_build.o</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="40">
                   <c:v>tx_timer_system_deactivate.o</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="41">
                   <c:v>tx_thread_initialize.o</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="42">
                   <c:v>tx_thread_timeout.o</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="43">
                   <c:v>stm32l4xx_hal_msp.o</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="44">
                   <c:v>tx_initialize_high_level.o</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="45">
                   <c:v>tx_timer_expiration_process.o</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="46">
                   <c:v>gpio.o</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="47">
                   <c:v>__scatter_zi.o</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="48">
                   <c:v>app_threadx.o</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="49">
                   <c:v>fz_wm.l</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="50">
                   <c:v>fpinit.o</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="51">
                   <c:v>__scatter_copy.o</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="52">
                   <c:v>exit.o</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="53">
                   <c:v>aeabi_memset.o</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="54">
                   <c:v>sys_exit.o</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="55">
                   <c:v>__rtentry2.o</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="56">
                   <c:v>stm32l4xx_it.o</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="57">
                   <c:v>rtexit2.o</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="58">
                   <c:v>libspace.o</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="59">
                   <c:v>__main.o</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="60">
                   <c:v>libinit2.o</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="61">
                   <c:v>heapauxi.o</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="62">
                   <c:v>__rtentry4.o</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="63">
                   <c:v>use_no_semi.o</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="64">
                   <c:v>rtexit.o</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="65">
                   <c:v>libshutdown2.o</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="66">
                   <c:v>libshutdown.o</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="67">
                   <c:v>libinit.o</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="68">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -663,194 +711,215 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flash_percent!$B$3:$B$64</c:f>
+              <c:f>flash_percent!$B$3:$B$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="62"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
-                  <c:v>26.84550285339356</c:v>
+                  <c:v>18.93583679199219</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.511496543884277</c:v>
+                  <c:v>15.26532936096191</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.840661525726318</c:v>
+                  <c:v>6.928439140319824</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.638967514038086</c:v>
+                  <c:v>6.003698825836182</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.013715267181397</c:v>
+                  <c:v>3.414425849914551</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.83219051361084</c:v>
+                  <c:v>3.272158145904541</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.590157270431519</c:v>
+                  <c:v>3.129890441894531</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.287616014480591</c:v>
+                  <c:v>2.831128120422363</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.20693826675415</c:v>
+                  <c:v>2.703087091445923</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.106091260910034</c:v>
+                  <c:v>2.532365798950195</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.783380508422852</c:v>
+                  <c:v>2.318964242935181</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.218636512756348</c:v>
+                  <c:v>2.262057304382324</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.855586886405945</c:v>
+                  <c:v>2.19092321395874</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.633723258972168</c:v>
+                  <c:v>1.963294863700867</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.613553881645203</c:v>
+                  <c:v>1.721439719200134</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.532876133918762</c:v>
+                  <c:v>1.564945220947266</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.472367882728577</c:v>
+                  <c:v>1.308863282203674</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.411859631538391</c:v>
+                  <c:v>1.152368783950806</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.351351380348206</c:v>
+                  <c:v>1.138141989707947</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.270673632621765</c:v>
+                  <c:v>1.081234931945801</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.129487752914429</c:v>
+                  <c:v>1.052781343460083</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.008471131324768</c:v>
+                  <c:v>1.038554549217224</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.9479628801345825</c:v>
+                  <c:v>1.038554549217224</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.9076240658760071</c:v>
+                  <c:v>0.9958742260932922</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.9076240658760071</c:v>
+                  <c:v>0.8962867856025696</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.8672851920127869</c:v>
+                  <c:v>0.7966994047164917</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.8471157550811768</c:v>
+                  <c:v>0.7397922873497009</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.7866075038909912</c:v>
+                  <c:v>0.668658435344696</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.7866075038909912</c:v>
+                  <c:v>0.6402048468589783</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.746268630027771</c:v>
+                  <c:v>0.6402048468589783</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.746268630027771</c:v>
+                  <c:v>0.6402048468589783</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.6857603788375855</c:v>
+                  <c:v>0.6117513179779053</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.64542156457901</c:v>
+                  <c:v>0.6117513179779053</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.5849132537841797</c:v>
+                  <c:v>0.5975245237350464</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.5849132537841797</c:v>
+                  <c:v>0.5548442006111145</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.5445744395256043</c:v>
+                  <c:v>0.5548442006111145</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.504235565662384</c:v>
+                  <c:v>0.5263906717300415</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.4638967216014862</c:v>
+                  <c:v>0.5263906717300415</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.3630496263504028</c:v>
+                  <c:v>0.4837103486061096</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.322710782289505</c:v>
+                  <c:v>0.4552567899227142</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.2823719382286072</c:v>
+                  <c:v>0.4125764667987824</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.2823719382286072</c:v>
+                  <c:v>0.4125764667987824</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.2622025012969971</c:v>
+                  <c:v>0.384122908115387</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.2622025012969971</c:v>
+                  <c:v>0.355669379234314</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.2622025012969971</c:v>
+                  <c:v>0.3272158205509186</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.1815248131752014</c:v>
+                  <c:v>0.2560819387435913</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.1613553911447525</c:v>
+                  <c:v>0.2276283949613571</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.1210165396332741</c:v>
+                  <c:v>0.1991748511791229</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.1210165396332741</c:v>
+                  <c:v>0.1991748511791229</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.1210165396332741</c:v>
+                  <c:v>0.1849480718374252</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.1008471176028252</c:v>
+                  <c:v>0.1849480718374252</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.08067769557237625</c:v>
+                  <c:v>0.1849480718374252</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.08067769557237625</c:v>
+                  <c:v>0.1280409693717957</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.06050826981663704</c:v>
+                  <c:v>0.1138141974806786</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.06050826981663704</c:v>
+                  <c:v>0.08536064624786377</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.06050826981663704</c:v>
+                  <c:v>0.08536064624786377</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.02016942389309406</c:v>
+                  <c:v>0.08536064624786377</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.02016942389309406</c:v>
+                  <c:v>0.07113387435674667</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.02016942389309406</c:v>
+                  <c:v>0.05690709874033928</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.02016942389309406</c:v>
+                  <c:v>0.05690709874033928</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.02016942389309406</c:v>
+                  <c:v>0.04268032312393189</c:v>
                 </c:pt>
                 <c:pt idx="61">
+                  <c:v>0.04268032312393189</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.04268032312393189</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.01422677468508482</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.01422677468508482</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.01422677468508482</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.01422677468508482</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.01422677468508482</c:v>
+                </c:pt>
+                <c:pt idx="68">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -955,8 +1024,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H64" totalsRowCount="1">
-  <autoFilter ref="A2:H63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H71" totalsRowCount="1">
+  <autoFilter ref="A2:H70"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="ram_percent" totalsRowFunction="sum"/>
@@ -972,8 +1041,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H64" totalsRowCount="1">
-  <autoFilter ref="A2:H63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H71" totalsRowCount="1">
+  <autoFilter ref="A2:H70"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="flash_percent" totalsRowFunction="sum"/>
@@ -1273,7 +1342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1289,28 +1358,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1318,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>33.3622932434082</v>
+        <v>32.76450347900391</v>
       </c>
       <c r="C3" s="1">
         <v>1536</v>
@@ -1344,16 +1413,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>26.06429100036621</v>
+        <v>25.59726905822754</v>
       </c>
       <c r="C4" s="1">
         <v>1200</v>
       </c>
       <c r="D4" s="1">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E4" s="1">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1370,7 +1439,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>18.85317039489746</v>
+        <v>18.51535797119141</v>
       </c>
       <c r="C5" s="1">
         <v>868</v>
@@ -1396,7 +1465,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>12.25021743774414</v>
+        <v>12.03071689605713</v>
       </c>
       <c r="C6" s="1">
         <v>564</v>
@@ -1422,7 +1491,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>3.735881805419922</v>
+        <v>3.668941974639893</v>
       </c>
       <c r="C7" s="1">
         <v>172</v>
@@ -1448,7 +1517,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>2.085143327713013</v>
+        <v>2.047781467437744</v>
       </c>
       <c r="C8" s="1">
         <v>96</v>
@@ -1474,7 +1543,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>2.085143327713013</v>
+        <v>2.047781467437744</v>
       </c>
       <c r="C9" s="1">
         <v>96</v>
@@ -1500,16 +1569,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>1.129452705383301</v>
+        <v>1.791808843612671</v>
       </c>
       <c r="C10" s="1">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="D10" s="1">
-        <v>46</v>
+        <v>242</v>
       </c>
       <c r="E10" s="1">
-        <v>46</v>
+        <v>242</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1518,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <v>52</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1526,25 +1595,25 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>0.2606429159641266</v>
+        <v>1.109215021133423</v>
       </c>
       <c r="C11" s="1">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D11" s="1">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="E11" s="1">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
       </c>
       <c r="G11" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1552,22 +1621,22 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>0.08688097447156906</v>
+        <v>0.255972683429718</v>
       </c>
       <c r="C12" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1">
-        <v>844</v>
+        <v>126</v>
       </c>
       <c r="E12" s="1">
-        <v>844</v>
+        <v>118</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H12" s="1">
         <v>4</v>
@@ -1578,56 +1647,82 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>0.08688097447156906</v>
+        <v>0.0853242352604866</v>
       </c>
       <c r="C13" s="1">
         <v>4</v>
       </c>
       <c r="D13" s="1">
+        <v>844</v>
+      </c>
+      <c r="E13" s="1">
+        <v>844</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.0853242352604866</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1">
         <v>86</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E14" s="1">
         <v>18</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F14" s="1">
         <v>64</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G14" s="1">
         <v>4</v>
       </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64">
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71">
         <f>SUBTOTAL(109,[ram_percent])</f>
         <v>0</v>
       </c>
-      <c r="C64">
+      <c r="C71">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="D64">
+      <c r="D71">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="E64">
+      <c r="E71">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F64">
+      <c r="F71">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G64">
+      <c r="G71">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H64">
+      <c r="H71">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>
@@ -1643,7 +1738,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1659,36 +1754,36 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
-        <v>26.84550285339356</v>
+        <v>18.93583679199219</v>
       </c>
       <c r="C3" s="1">
         <v>2662</v>
@@ -1711,19 +1806,19 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
-        <v>8.511496543884277</v>
+        <v>15.26532936096191</v>
       </c>
       <c r="C4" s="1">
-        <v>844</v>
+        <v>2146</v>
       </c>
       <c r="D4" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>844</v>
+        <v>2146</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1732,24 +1827,24 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
-        <v>4.840661525726318</v>
+        <v>6.928439140319824</v>
       </c>
       <c r="C5" s="1">
-        <v>480</v>
+        <v>974</v>
       </c>
       <c r="D5" s="1">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>480</v>
+        <v>974</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -1758,50 +1853,50 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2">
-        <v>4.638967514038086</v>
+        <v>6.003698825836182</v>
       </c>
       <c r="C6" s="1">
-        <v>460</v>
+        <v>844</v>
       </c>
       <c r="D6" s="1">
-        <v>1536</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
-        <v>64</v>
+        <v>844</v>
       </c>
       <c r="F6" s="1">
-        <v>396</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <v>1536</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>4.013715267181397</v>
+        <v>3.414425849914551</v>
       </c>
       <c r="C7" s="1">
-        <v>398</v>
+        <v>480</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="E7" s="1">
-        <v>398</v>
+        <v>480</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -1810,50 +1905,50 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2">
-        <v>3.83219051361084</v>
+        <v>3.272158145904541</v>
       </c>
       <c r="C8" s="1">
-        <v>380</v>
+        <v>460</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>1536</v>
       </c>
       <c r="E8" s="1">
-        <v>380</v>
+        <v>64</v>
       </c>
       <c r="F8" s="1">
-        <v>0</v>
+        <v>396</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2">
-        <v>3.590157270431519</v>
+        <v>3.129890441894531</v>
       </c>
       <c r="C9" s="1">
-        <v>356</v>
+        <v>440</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>356</v>
+        <v>440</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1867,19 +1962,19 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2">
-        <v>3.287616014480591</v>
+        <v>2.831128120422363</v>
       </c>
       <c r="C10" s="1">
-        <v>326</v>
+        <v>398</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>326</v>
+        <v>398</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1893,19 +1988,19 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2">
-        <v>3.20693826675415</v>
+        <v>2.703087091445923</v>
       </c>
       <c r="C11" s="1">
-        <v>318</v>
+        <v>380</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>318</v>
+        <v>380</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1919,19 +2014,19 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2">
-        <v>3.106091260910034</v>
+        <v>2.532365798950195</v>
       </c>
       <c r="C12" s="1">
-        <v>308</v>
+        <v>356</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>308</v>
+        <v>356</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1945,19 +2040,19 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2">
-        <v>2.783380508422852</v>
+        <v>2.318964242935181</v>
       </c>
       <c r="C13" s="1">
-        <v>276</v>
+        <v>326</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>276</v>
+        <v>326</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1971,19 +2066,19 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2">
-        <v>2.218636512756348</v>
+        <v>2.262057304382324</v>
       </c>
       <c r="C14" s="1">
-        <v>220</v>
+        <v>318</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>220</v>
+        <v>318</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -1997,19 +2092,19 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2">
-        <v>1.855586886405945</v>
+        <v>2.19092321395874</v>
       </c>
       <c r="C15" s="1">
-        <v>184</v>
+        <v>308</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>184</v>
+        <v>308</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -2023,19 +2118,19 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2">
-        <v>1.633723258972168</v>
+        <v>1.963294863700867</v>
       </c>
       <c r="C16" s="1">
-        <v>162</v>
+        <v>276</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>162</v>
+        <v>276</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -2049,19 +2144,19 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2">
-        <v>1.613553881645203</v>
+        <v>1.721439719200134</v>
       </c>
       <c r="C17" s="1">
-        <v>160</v>
+        <v>242</v>
       </c>
       <c r="D17" s="1">
-        <v>868</v>
+        <v>84</v>
       </c>
       <c r="E17" s="1">
-        <v>160</v>
+        <v>242</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -2070,24 +2165,24 @@
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <v>868</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2">
-        <v>1.532876133918762</v>
+        <v>1.564945220947266</v>
       </c>
       <c r="C18" s="1">
-        <v>152</v>
+        <v>220</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>152</v>
+        <v>220</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
@@ -2101,19 +2196,19 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2">
-        <v>1.472367882728577</v>
+        <v>1.308863282203674</v>
       </c>
       <c r="C19" s="1">
-        <v>146</v>
+        <v>184</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>146</v>
+        <v>184</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -2127,19 +2222,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2">
-        <v>1.411859631538391</v>
+        <v>1.152368783950806</v>
       </c>
       <c r="C20" s="1">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -2153,19 +2248,19 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B21" s="2">
-        <v>1.351351380348206</v>
+        <v>1.138141989707947</v>
       </c>
       <c r="C21" s="1">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>868</v>
       </c>
       <c r="E21" s="1">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -2174,50 +2269,50 @@
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <v>0</v>
+        <v>868</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2">
-        <v>1.270673632621765</v>
+        <v>1.081234931945801</v>
       </c>
       <c r="C22" s="1">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="D22" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
       </c>
       <c r="G22" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2">
-        <v>1.129487752914429</v>
+        <v>1.052781343460083</v>
       </c>
       <c r="C23" s="1">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -2231,19 +2326,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2">
-        <v>1.008471131324768</v>
+        <v>1.038554549217224</v>
       </c>
       <c r="C24" s="1">
-        <v>100</v>
+        <v>146</v>
       </c>
       <c r="D24" s="1">
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>100</v>
+        <v>146</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -2252,24 +2347,24 @@
         <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>1200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2">
-        <v>0.9479628801345825</v>
+        <v>1.038554549217224</v>
       </c>
       <c r="C25" s="1">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -2283,19 +2378,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2">
-        <v>0.9076240658760071</v>
+        <v>0.9958742260932922</v>
       </c>
       <c r="C26" s="1">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -2309,51 +2404,51 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B27" s="2">
-        <v>0.9076240658760071</v>
+        <v>0.8962867856025696</v>
       </c>
       <c r="C27" s="1">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E27" s="1">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
       </c>
       <c r="G27" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H27" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2">
-        <v>0.8672851920127869</v>
+        <v>0.7966994047164917</v>
       </c>
       <c r="C28" s="1">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="D28" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="F28" s="1">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="G28" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H28" s="1">
         <v>0</v>
@@ -2361,19 +2456,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B29" s="2">
-        <v>0.8471157550811768</v>
+        <v>0.7397922873497009</v>
       </c>
       <c r="C29" s="1">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="D29" s="1">
-        <v>564</v>
+        <v>1200</v>
       </c>
       <c r="E29" s="1">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -2382,24 +2477,24 @@
         <v>0</v>
       </c>
       <c r="H29" s="1">
-        <v>564</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B30" s="2">
-        <v>0.7866075038909912</v>
+        <v>0.668658435344696</v>
       </c>
       <c r="C30" s="1">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -2413,19 +2508,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B31" s="2">
-        <v>0.7866075038909912</v>
+        <v>0.6402048468589783</v>
       </c>
       <c r="C31" s="1">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -2439,19 +2534,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B32" s="2">
-        <v>0.746268630027771</v>
+        <v>0.6402048468589783</v>
       </c>
       <c r="C32" s="1">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -2465,19 +2560,19 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B33" s="2">
-        <v>0.746268630027771</v>
+        <v>0.6402048468589783</v>
       </c>
       <c r="C33" s="1">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
@@ -2491,25 +2586,25 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B34" s="2">
-        <v>0.6857603788375855</v>
+        <v>0.6117513179779053</v>
       </c>
       <c r="C34" s="1">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="D34" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E34" s="1">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="F34" s="1">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="G34" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H34" s="1">
         <v>0</v>
@@ -2517,19 +2612,19 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2">
-        <v>0.64542156457901</v>
+        <v>0.6117513179779053</v>
       </c>
       <c r="C35" s="1">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
@@ -2543,19 +2638,19 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B36" s="2">
-        <v>0.5849132537841797</v>
+        <v>0.5975245237350464</v>
       </c>
       <c r="C36" s="1">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="D36" s="1">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="E36" s="1">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
@@ -2564,50 +2659,50 @@
         <v>0</v>
       </c>
       <c r="H36" s="1">
-        <v>0</v>
+        <v>564</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B37" s="2">
-        <v>0.5849132537841797</v>
+        <v>0.5548442006111145</v>
       </c>
       <c r="C37" s="1">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="D37" s="1">
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
       </c>
       <c r="G37" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H37" s="1">
-        <v>168</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B38" s="2">
-        <v>0.5445744395256043</v>
+        <v>0.5548442006111145</v>
       </c>
       <c r="C38" s="1">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
       </c>
       <c r="E38" s="1">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
@@ -2621,19 +2716,19 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B39" s="2">
-        <v>0.504235565662384</v>
+        <v>0.5263906717300415</v>
       </c>
       <c r="C39" s="1">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F39" s="1">
         <v>0</v>
@@ -2647,19 +2742,19 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B40" s="2">
-        <v>0.4638967216014862</v>
+        <v>0.5263906717300415</v>
       </c>
       <c r="C40" s="1">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="D40" s="1">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E40" s="1">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
@@ -2668,24 +2763,24 @@
         <v>0</v>
       </c>
       <c r="H40" s="1">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B41" s="2">
-        <v>0.3630496263504028</v>
+        <v>0.4837103486061096</v>
       </c>
       <c r="C41" s="1">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
@@ -2699,19 +2794,19 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B42" s="2">
-        <v>0.322710782289505</v>
+        <v>0.4552567899227142</v>
       </c>
       <c r="C42" s="1">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="F42" s="1">
         <v>0</v>
@@ -2725,19 +2820,19 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B43" s="2">
-        <v>0.2823719382286072</v>
+        <v>0.4125764667987824</v>
       </c>
       <c r="C43" s="1">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
       </c>
       <c r="E43" s="1">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="F43" s="1">
         <v>0</v>
@@ -2751,45 +2846,45 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B44" s="2">
-        <v>0.2823719382286072</v>
+        <v>0.4125764667987824</v>
       </c>
       <c r="C44" s="1">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D44" s="1">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="E44" s="1">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="F44" s="1">
         <v>0</v>
       </c>
       <c r="G44" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H44" s="1">
-        <v>0</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" s="2">
-        <v>0.2622025012969971</v>
+        <v>0.384122908115387</v>
       </c>
       <c r="C45" s="1">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="D45" s="1">
         <v>0</v>
       </c>
       <c r="E45" s="1">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="F45" s="1">
         <v>0</v>
@@ -2803,19 +2898,19 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" s="2">
-        <v>0.2622025012969971</v>
+        <v>0.355669379234314</v>
       </c>
       <c r="C46" s="1">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
       </c>
       <c r="E46" s="1">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="F46" s="1">
         <v>0</v>
@@ -2829,19 +2924,19 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0.3272158205509186</v>
+      </c>
+      <c r="C47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="2">
-        <v>0.2622025012969971</v>
-      </c>
-      <c r="C47" s="1">
-        <v>26</v>
-      </c>
       <c r="D47" s="1">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E47" s="1">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="F47" s="1">
         <v>0</v>
@@ -2850,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="H47" s="1">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2858,16 +2953,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="2">
-        <v>0.1815248131752014</v>
+        <v>0.2560819387435913</v>
       </c>
       <c r="C48" s="1">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
       </c>
       <c r="E48" s="1">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F48" s="1">
         <v>0</v>
@@ -2884,16 +2979,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="2">
-        <v>0.1613553911447525</v>
+        <v>0.2276283949613571</v>
       </c>
       <c r="C49" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
       </c>
       <c r="E49" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F49" s="1">
         <v>0</v>
@@ -2910,16 +3005,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="2">
-        <v>0.1210165396332741</v>
+        <v>0.1991748511791229</v>
       </c>
       <c r="C50" s="1">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D50" s="1">
         <v>0</v>
       </c>
       <c r="E50" s="1">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F50" s="1">
         <v>0</v>
@@ -2936,16 +3031,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="2">
-        <v>0.1210165396332741</v>
+        <v>0.1991748511791229</v>
       </c>
       <c r="C51" s="1">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
       </c>
       <c r="E51" s="1">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
@@ -2962,16 +3057,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="2">
-        <v>0.1210165396332741</v>
+        <v>0.1849480718374252</v>
       </c>
       <c r="C52" s="1">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D52" s="1">
         <v>0</v>
       </c>
       <c r="E52" s="1">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F52" s="1">
         <v>0</v>
@@ -2988,16 +3083,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>0.1008471176028252</v>
+        <v>0.1849480718374252</v>
       </c>
       <c r="C53" s="1">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
       </c>
       <c r="E53" s="1">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F53" s="1">
         <v>0</v>
@@ -3011,19 +3106,19 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>0.08067769557237625</v>
+        <v>0.1849480718374252</v>
       </c>
       <c r="C54" s="1">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D54" s="1">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="E54" s="1">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F54" s="1">
         <v>0</v>
@@ -3032,24 +3127,24 @@
         <v>0</v>
       </c>
       <c r="H54" s="1">
-        <v>96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B55" s="2">
-        <v>0.08067769557237625</v>
+        <v>0.1280409693717957</v>
       </c>
       <c r="C55" s="1">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
       </c>
       <c r="E55" s="1">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F55" s="1">
         <v>0</v>
@@ -3063,19 +3158,19 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56" s="2">
-        <v>0.06050826981663704</v>
+        <v>0.1138141974806786</v>
       </c>
       <c r="C56" s="1">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
       </c>
       <c r="E56" s="1">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
@@ -3089,19 +3184,19 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B57" s="2">
-        <v>0.06050826981663704</v>
+        <v>0.08536064624786377</v>
       </c>
       <c r="C57" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
       </c>
       <c r="E57" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
@@ -3115,19 +3210,19 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>0.06050826981663704</v>
+        <v>0.08536064624786377</v>
       </c>
       <c r="C58" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D58" s="1">
         <v>0</v>
       </c>
       <c r="E58" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F58" s="1">
         <v>0</v>
@@ -3141,19 +3236,19 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B59" s="2">
-        <v>0.02016942389309406</v>
+        <v>0.08536064624786377</v>
       </c>
       <c r="C59" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
       </c>
       <c r="E59" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F59" s="1">
         <v>0</v>
@@ -3167,19 +3262,19 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>0.02016942389309406</v>
+        <v>0.07113387435674667</v>
       </c>
       <c r="C60" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D60" s="1">
         <v>0</v>
       </c>
       <c r="E60" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F60" s="1">
         <v>0</v>
@@ -3193,19 +3288,19 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="B61" s="2">
-        <v>0.02016942389309406</v>
+        <v>0.05690709874033928</v>
       </c>
       <c r="C61" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D61" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="E61" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F61" s="1">
         <v>0</v>
@@ -3214,7 +3309,7 @@
         <v>0</v>
       </c>
       <c r="H61" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3222,16 +3317,16 @@
         <v>60</v>
       </c>
       <c r="B62" s="2">
-        <v>0.02016942389309406</v>
+        <v>0.05690709874033928</v>
       </c>
       <c r="C62" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D62" s="1">
         <v>0</v>
       </c>
       <c r="E62" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F62" s="1">
         <v>0</v>
@@ -3248,56 +3343,238 @@
         <v>61</v>
       </c>
       <c r="B63" s="2">
-        <v>0.02016942389309406</v>
+        <v>0.04268032312393189</v>
       </c>
       <c r="C63" s="1">
+        <v>6</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1">
+        <v>6</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" s="2">
+        <v>0.04268032312393189</v>
+      </c>
+      <c r="C64" s="1">
+        <v>6</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1">
+        <v>6</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0.04268032312393189</v>
+      </c>
+      <c r="C65" s="1">
+        <v>6</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>6</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" s="2">
+        <v>0.01422677468508482</v>
+      </c>
+      <c r="C66" s="1">
         <v>2</v>
       </c>
-      <c r="D63" s="1">
-        <v>0</v>
-      </c>
-      <c r="E63" s="1">
+      <c r="D66" s="1">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1">
         <v>2</v>
       </c>
-      <c r="F63" s="1">
-        <v>0</v>
-      </c>
-      <c r="G63" s="1">
-        <v>0</v>
-      </c>
-      <c r="H63" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64">
+      <c r="F66" s="1">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1">
+        <v>0</v>
+      </c>
+      <c r="H66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2">
+        <v>0.01422677468508482</v>
+      </c>
+      <c r="C67" s="1">
+        <v>2</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1">
+        <v>2</v>
+      </c>
+      <c r="F67" s="1">
+        <v>0</v>
+      </c>
+      <c r="G67" s="1">
+        <v>0</v>
+      </c>
+      <c r="H67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" s="2">
+        <v>0.01422677468508482</v>
+      </c>
+      <c r="C68" s="1">
+        <v>2</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1">
+        <v>2</v>
+      </c>
+      <c r="F68" s="1">
+        <v>0</v>
+      </c>
+      <c r="G68" s="1">
+        <v>0</v>
+      </c>
+      <c r="H68" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" s="2">
+        <v>0.01422677468508482</v>
+      </c>
+      <c r="C69" s="1">
+        <v>2</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1">
+        <v>2</v>
+      </c>
+      <c r="F69" s="1">
+        <v>0</v>
+      </c>
+      <c r="G69" s="1">
+        <v>0</v>
+      </c>
+      <c r="H69" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B70" s="2">
+        <v>0.01422677468508482</v>
+      </c>
+      <c r="C70" s="1">
+        <v>2</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1">
+        <v>2</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1">
+        <v>0</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71">
         <f>SUBTOTAL(109,[flash_percent])</f>
         <v>0</v>
       </c>
-      <c r="C64">
+      <c r="C71">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="D64">
+      <c r="D71">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="E64">
+      <c r="E71">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F64">
+      <c r="F71">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G64">
+      <c r="G71">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H64">
+      <c r="H71">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Add RX8900 set and update time api
</commit_message>
<xml_diff>
--- a/Software/MDK-ARM/Software_analysis.xlsx
+++ b/Software/MDK-ARM/Software_analysis.xlsx
@@ -396,43 +396,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="69"/>
                 <c:pt idx="0">
-                  <c:v>32.60454177856445</c:v>
+                  <c:v>32.55616760253906</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.47229957580566</c:v>
+                  <c:v>25.5828742980957</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.42496299743652</c:v>
+                  <c:v>18.39762687683106</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.97198009490967</c:v>
+                  <c:v>11.9542179107666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.651029586791992</c:v>
+                  <c:v>3.645612478256226</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.037783861160278</c:v>
+                  <c:v>2.034760475158691</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.037783861160278</c:v>
+                  <c:v>2.034760475158691</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.783060908317566</c:v>
+                  <c:v>1.780415415763855</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.10379958152771</c:v>
+                  <c:v>1.102161884307861</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.4882190525531769</c:v>
+                  <c:v>0.487494707107544</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2547229826450348</c:v>
+                  <c:v>0.2543450593948364</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.084907665848732</c:v>
+                  <c:v>0.08478168398141861</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.084907665848732</c:v>
+                  <c:v>0.08478168398141861</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>0</c:v>
@@ -518,76 +518,76 @@
                   <c:v>tx_low_power.o</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>rx8900.o</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>c_w.l</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>startup_stm32l432xx.o</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>stm32l4xx_hal_gpio.o</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>txe_thread_create.o</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>tx_thread_system_suspend.o</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>txe_byte_pool_create.o</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>tx_timer_thread_entry.o</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>tx_thread_create.o</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>tx_thread_system_resume.o</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>stm32l4xx_hal_pwr_ex.o</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>i2c.o</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>tx_thread_schedule.o</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>tx_timer_interrupt.o</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>stm32l4xx_hal_cortex.o</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>tx_timer_initialize.o</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>tx_initialize_low_level.o</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
+                  <c:v>appmain.o</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>main.o</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>tx_thread_sleep.o</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>stm32l4xx_hal_i2c_ex.o</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>tx_byte_pool_create.o</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>stm32l4xx_hal.o</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>tx_thread_time_slice.o</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>rx8900.o</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>appmain.o</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>__scatter.o</c:v>
@@ -722,208 +722,208 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="69"/>
                 <c:pt idx="0">
-                  <c:v>18.9102783203125</c:v>
+                  <c:v>18.06583023071289</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.24472522735596</c:v>
+                  <c:v>14.56396293640137</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.919087886810303</c:v>
+                  <c:v>6.610112190246582</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.995595455169678</c:v>
+                  <c:v>5.727859020233154</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.409817457199097</c:v>
+                  <c:v>4.865965366363525</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.267741680145264</c:v>
+                  <c:v>3.257550001144409</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.125665903091431</c:v>
+                  <c:v>3.121818780899048</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.827306985855103</c:v>
+                  <c:v>2.986087560653687</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.699438810348511</c:v>
+                  <c:v>2.701051950454712</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.528947830200195</c:v>
+                  <c:v>2.578893899917603</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.315834283828735</c:v>
+                  <c:v>2.416016340255737</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.25900411605835</c:v>
+                  <c:v>2.212419509887695</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.187966108322144</c:v>
+                  <c:v>2.158126831054688</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.960645079612732</c:v>
+                  <c:v>2.090261220932007</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.71911633014679</c:v>
+                  <c:v>1.873091220855713</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.562832951545715</c:v>
+                  <c:v>1.642348170280457</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.307096719741821</c:v>
+                  <c:v>1.493043780326843</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.150813341140747</c:v>
+                  <c:v>1.248727560043335</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.136605858802795</c:v>
+                  <c:v>1.099423170089722</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.07977557182312</c:v>
+                  <c:v>1.08585000038147</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.051360368728638</c:v>
+                  <c:v>1.031557559967041</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.037152767181397</c:v>
+                  <c:v>1.017984390258789</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.037152767181397</c:v>
+                  <c:v>1.004411220550537</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.9945300817489624</c:v>
+                  <c:v>0.9908381700515747</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.8950770497322083</c:v>
+                  <c:v>0.9908381700515747</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.7956240773200989</c:v>
+                  <c:v>0.9501187801361084</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.7458975911140442</c:v>
+                  <c:v>0.8551068902015686</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.7387937903404236</c:v>
+                  <c:v>0.7600950002670288</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.6677559018135071</c:v>
+                  <c:v>0.6379368901252747</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.6393407583236694</c:v>
+                  <c:v>0.6107906103134155</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.6393407583236694</c:v>
+                  <c:v>0.6107906103134155</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.6393407583236694</c:v>
+                  <c:v>0.6107906103134155</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.6109256148338318</c:v>
+                  <c:v>0.5836443901062012</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.5967180728912354</c:v>
+                  <c:v>0.570071280002594</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.5540953278541565</c:v>
+                  <c:v>0.5293518900871277</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.5540953278541565</c:v>
+                  <c:v>0.5293518900871277</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.5256801843643189</c:v>
+                  <c:v>0.5022056102752686</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.5256801843643189</c:v>
+                  <c:v>0.5022056102752686</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.4830574691295624</c:v>
+                  <c:v>0.4614862501621246</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.4546423256397247</c:v>
+                  <c:v>0.4343400001525879</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.4120196104049683</c:v>
+                  <c:v>0.393620640039444</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.4120196104049683</c:v>
+                  <c:v>0.393620640039444</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.3836044669151306</c:v>
+                  <c:v>0.3664743900299072</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.355189323425293</c:v>
+                  <c:v>0.3393281400203705</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.3267741799354553</c:v>
+                  <c:v>0.3121818900108337</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.2557363212108612</c:v>
+                  <c:v>0.2443162500858307</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.2273211628198624</c:v>
+                  <c:v>0.217170000076294</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.1989060193300247</c:v>
+                  <c:v>0.1900237500667572</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.1989060193300247</c:v>
+                  <c:v>0.1900237500667572</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.1846984475851059</c:v>
+                  <c:v>0.1764506250619888</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.1846984475851059</c:v>
+                  <c:v>0.1764506250619888</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.1846984475851059</c:v>
+                  <c:v>0.1764506250619888</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.1278681606054306</c:v>
+                  <c:v>0.1221581250429153</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.1136605814099312</c:v>
+                  <c:v>0.108585000038147</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.08524543792009354</c:v>
+                  <c:v>0.08143875002861023</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.08524543792009354</c:v>
+                  <c:v>0.08143875002861023</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.08524543792009354</c:v>
+                  <c:v>0.08143875002861023</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.07103786617517471</c:v>
+                  <c:v>0.06786562502384186</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.05683029070496559</c:v>
+                  <c:v>0.05429250001907349</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.05683029070496559</c:v>
+                  <c:v>0.05429250001907349</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.04262271896004677</c:v>
+                  <c:v>0.04071937501430512</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.04262271896004677</c:v>
+                  <c:v>0.04071937501430512</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.04262271896004677</c:v>
+                  <c:v>0.04071937501430512</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.0142075726762414</c:v>
+                  <c:v>0.01357312500476837</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.0142075726762414</c:v>
+                  <c:v>0.01357312500476837</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.0142075726762414</c:v>
+                  <c:v>0.01357312500476837</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.0142075726762414</c:v>
+                  <c:v>0.01357312500476837</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.0142075726762414</c:v>
+                  <c:v>0.01357312500476837</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>0</c:v>
@@ -1393,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>32.60454177856445</v>
+        <v>32.55616760253906</v>
       </c>
       <c r="C3" s="1">
         <v>1536</v>
@@ -1419,16 +1419,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>25.47229957580566</v>
+        <v>25.5828742980957</v>
       </c>
       <c r="C4" s="1">
-        <v>1200</v>
+        <v>1207</v>
       </c>
       <c r="D4" s="1">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="E4" s="1">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1437,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>1200</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1445,7 +1445,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>18.42496299743652</v>
+        <v>18.39762687683106</v>
       </c>
       <c r="C5" s="1">
         <v>868</v>
@@ -1471,7 +1471,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>11.97198009490967</v>
+        <v>11.9542179107666</v>
       </c>
       <c r="C6" s="1">
         <v>564</v>
@@ -1497,7 +1497,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>3.651029586791992</v>
+        <v>3.645612478256226</v>
       </c>
       <c r="C7" s="1">
         <v>172</v>
@@ -1523,7 +1523,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>2.037783861160278</v>
+        <v>2.034760475158691</v>
       </c>
       <c r="C8" s="1">
         <v>96</v>
@@ -1549,7 +1549,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>2.037783861160278</v>
+        <v>2.034760475158691</v>
       </c>
       <c r="C9" s="1">
         <v>96</v>
@@ -1575,7 +1575,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>1.783060908317566</v>
+        <v>1.780415415763855</v>
       </c>
       <c r="C10" s="1">
         <v>84</v>
@@ -1601,7 +1601,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>1.10379958152771</v>
+        <v>1.102161884307861</v>
       </c>
       <c r="C11" s="1">
         <v>52</v>
@@ -1627,16 +1627,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>0.4882190525531769</v>
+        <v>0.487494707107544</v>
       </c>
       <c r="C12" s="1">
         <v>23</v>
       </c>
       <c r="D12" s="1">
-        <v>105</v>
+        <v>717</v>
       </c>
       <c r="E12" s="1">
-        <v>104</v>
+        <v>716</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1653,7 +1653,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>0.2547229826450348</v>
+        <v>0.2543450593948364</v>
       </c>
       <c r="C13" s="1">
         <v>12</v>
@@ -1679,7 +1679,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>0.084907665848732</v>
+        <v>0.08478168398141861</v>
       </c>
       <c r="C14" s="1">
         <v>4</v>
@@ -1705,7 +1705,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>0.084907665848732</v>
+        <v>0.08478168398141861</v>
       </c>
       <c r="C15" s="1">
         <v>4</v>
@@ -1815,7 +1815,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="2">
-        <v>18.9102783203125</v>
+        <v>18.06583023071289</v>
       </c>
       <c r="C3" s="1">
         <v>2662</v>
@@ -1841,7 +1841,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="2">
-        <v>15.24472522735596</v>
+        <v>14.56396293640137</v>
       </c>
       <c r="C4" s="1">
         <v>2146</v>
@@ -1867,7 +1867,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="2">
-        <v>6.919087886810303</v>
+        <v>6.610112190246582</v>
       </c>
       <c r="C5" s="1">
         <v>974</v>
@@ -1893,7 +1893,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2">
-        <v>5.995595455169678</v>
+        <v>5.727859020233154</v>
       </c>
       <c r="C6" s="1">
         <v>844</v>
@@ -1916,97 +1916,97 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>3.409817457199097</v>
+        <v>4.865965366363525</v>
       </c>
       <c r="C7" s="1">
-        <v>480</v>
+        <v>717</v>
       </c>
       <c r="D7" s="1">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1">
-        <v>480</v>
+        <v>716</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1">
-        <v>96</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>3.267741680145264</v>
+        <v>3.257550001144409</v>
       </c>
       <c r="C8" s="1">
-        <v>460</v>
+        <v>480</v>
       </c>
       <c r="D8" s="1">
-        <v>1536</v>
+        <v>96</v>
       </c>
       <c r="E8" s="1">
-        <v>64</v>
+        <v>480</v>
       </c>
       <c r="F8" s="1">
-        <v>396</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>1536</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B9" s="2">
-        <v>3.125665903091431</v>
+        <v>3.121818780899048</v>
       </c>
       <c r="C9" s="1">
-        <v>440</v>
+        <v>460</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>1536</v>
       </c>
       <c r="E9" s="1">
-        <v>440</v>
+        <v>64</v>
       </c>
       <c r="F9" s="1">
-        <v>0</v>
+        <v>396</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2">
-        <v>2.827306985855103</v>
+        <v>2.986087560653687</v>
       </c>
       <c r="C10" s="1">
-        <v>398</v>
+        <v>440</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>398</v>
+        <v>440</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -2020,19 +2020,19 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2">
-        <v>2.699438810348511</v>
+        <v>2.701051950454712</v>
       </c>
       <c r="C11" s="1">
-        <v>380</v>
+        <v>398</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>380</v>
+        <v>398</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -2046,19 +2046,19 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2">
-        <v>2.528947830200195</v>
+        <v>2.578893899917603</v>
       </c>
       <c r="C12" s="1">
-        <v>356</v>
+        <v>380</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>356</v>
+        <v>380</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -2072,19 +2072,19 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2">
-        <v>2.315834283828735</v>
+        <v>2.416016340255737</v>
       </c>
       <c r="C13" s="1">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -2098,19 +2098,19 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2">
-        <v>2.25900411605835</v>
+        <v>2.212419509887695</v>
       </c>
       <c r="C14" s="1">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -2124,19 +2124,19 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2">
-        <v>2.187966108322144</v>
+        <v>2.158126831054688</v>
       </c>
       <c r="C15" s="1">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -2150,19 +2150,19 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2">
-        <v>1.960645079612732</v>
+        <v>2.090261220932007</v>
       </c>
       <c r="C16" s="1">
-        <v>276</v>
+        <v>308</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>276</v>
+        <v>308</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -2176,19 +2176,19 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2">
-        <v>1.71911633014679</v>
+        <v>1.873091220855713</v>
       </c>
       <c r="C17" s="1">
-        <v>242</v>
+        <v>276</v>
       </c>
       <c r="D17" s="1">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>242</v>
+        <v>276</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -2197,24 +2197,24 @@
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <v>84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B18" s="2">
-        <v>1.562832951545715</v>
+        <v>1.642348170280457</v>
       </c>
       <c r="C18" s="1">
-        <v>220</v>
+        <v>242</v>
       </c>
       <c r="D18" s="1">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="E18" s="1">
-        <v>220</v>
+        <v>242</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
@@ -2223,24 +2223,24 @@
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2">
-        <v>1.307096719741821</v>
+        <v>1.493043780326843</v>
       </c>
       <c r="C19" s="1">
-        <v>184</v>
+        <v>220</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>184</v>
+        <v>220</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -2254,19 +2254,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2">
-        <v>1.150813341140747</v>
+        <v>1.248727560043335</v>
       </c>
       <c r="C20" s="1">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -2280,19 +2280,19 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2">
-        <v>1.136605858802795</v>
+        <v>1.099423170089722</v>
       </c>
       <c r="C21" s="1">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D21" s="1">
-        <v>868</v>
+        <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -2301,24 +2301,24 @@
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <v>868</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="B22" s="2">
-        <v>1.07977557182312</v>
+        <v>1.08585000038147</v>
       </c>
       <c r="C22" s="1">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="D22" s="1">
-        <v>0</v>
+        <v>868</v>
       </c>
       <c r="E22" s="1">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -2327,24 +2327,24 @@
         <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>0</v>
+        <v>868</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2">
-        <v>1.051360368728638</v>
+        <v>1.031557559967041</v>
       </c>
       <c r="C23" s="1">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -2358,19 +2358,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="B24" s="2">
-        <v>1.037152767181397</v>
+        <v>1.017984390258789</v>
       </c>
       <c r="C24" s="1">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D24" s="1">
-        <v>0</v>
+        <v>1207</v>
       </c>
       <c r="E24" s="1">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -2379,24 +2379,24 @@
         <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>0</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2">
-        <v>1.037152767181397</v>
+        <v>1.004411220550537</v>
       </c>
       <c r="C25" s="1">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -2410,19 +2410,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2">
-        <v>0.9945300817489624</v>
+        <v>0.9908381700515747</v>
       </c>
       <c r="C26" s="1">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -2436,45 +2436,45 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B27" s="2">
-        <v>0.8950770497322083</v>
+        <v>0.9908381700515747</v>
       </c>
       <c r="C27" s="1">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="D27" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
       </c>
       <c r="G27" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H27" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2">
-        <v>0.7956240773200989</v>
+        <v>0.9501187801361084</v>
       </c>
       <c r="C28" s="1">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -2488,45 +2488,45 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B29" s="2">
-        <v>0.7458975911140442</v>
+        <v>0.8551068902015686</v>
       </c>
       <c r="C29" s="1">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="D29" s="1">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E29" s="1">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
       </c>
       <c r="G29" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H29" s="1">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B30" s="2">
-        <v>0.7387937903404236</v>
+        <v>0.7600950002670288</v>
       </c>
       <c r="C30" s="1">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D30" s="1">
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -2535,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="1">
-        <v>1200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2543,7 +2543,7 @@
         <v>34</v>
       </c>
       <c r="B31" s="2">
-        <v>0.6677559018135071</v>
+        <v>0.6379368901252747</v>
       </c>
       <c r="C31" s="1">
         <v>94</v>
@@ -2569,7 +2569,7 @@
         <v>35</v>
       </c>
       <c r="B32" s="2">
-        <v>0.6393407583236694</v>
+        <v>0.6107906103134155</v>
       </c>
       <c r="C32" s="1">
         <v>90</v>
@@ -2595,7 +2595,7 @@
         <v>36</v>
       </c>
       <c r="B33" s="2">
-        <v>0.6393407583236694</v>
+        <v>0.6107906103134155</v>
       </c>
       <c r="C33" s="1">
         <v>90</v>
@@ -2621,7 +2621,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="2">
-        <v>0.6393407583236694</v>
+        <v>0.6107906103134155</v>
       </c>
       <c r="C34" s="1">
         <v>90</v>
@@ -2647,7 +2647,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="2">
-        <v>0.6109256148338318</v>
+        <v>0.5836443901062012</v>
       </c>
       <c r="C35" s="1">
         <v>86</v>
@@ -2673,7 +2673,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="2">
-        <v>0.5967180728912354</v>
+        <v>0.570071280002594</v>
       </c>
       <c r="C36" s="1">
         <v>84</v>
@@ -2699,7 +2699,7 @@
         <v>38</v>
       </c>
       <c r="B37" s="2">
-        <v>0.5540953278541565</v>
+        <v>0.5293518900871277</v>
       </c>
       <c r="C37" s="1">
         <v>78</v>
@@ -2725,7 +2725,7 @@
         <v>39</v>
       </c>
       <c r="B38" s="2">
-        <v>0.5540953278541565</v>
+        <v>0.5293518900871277</v>
       </c>
       <c r="C38" s="1">
         <v>78</v>
@@ -2751,7 +2751,7 @@
         <v>40</v>
       </c>
       <c r="B39" s="2">
-        <v>0.5256801843643189</v>
+        <v>0.5022056102752686</v>
       </c>
       <c r="C39" s="1">
         <v>74</v>
@@ -2777,7 +2777,7 @@
         <v>41</v>
       </c>
       <c r="B40" s="2">
-        <v>0.5256801843643189</v>
+        <v>0.5022056102752686</v>
       </c>
       <c r="C40" s="1">
         <v>74</v>
@@ -2803,7 +2803,7 @@
         <v>42</v>
       </c>
       <c r="B41" s="2">
-        <v>0.4830574691295624</v>
+        <v>0.4614862501621246</v>
       </c>
       <c r="C41" s="1">
         <v>68</v>
@@ -2829,7 +2829,7 @@
         <v>43</v>
       </c>
       <c r="B42" s="2">
-        <v>0.4546423256397247</v>
+        <v>0.4343400001525879</v>
       </c>
       <c r="C42" s="1">
         <v>64</v>
@@ -2855,7 +2855,7 @@
         <v>44</v>
       </c>
       <c r="B43" s="2">
-        <v>0.4120196104049683</v>
+        <v>0.393620640039444</v>
       </c>
       <c r="C43" s="1">
         <v>58</v>
@@ -2881,7 +2881,7 @@
         <v>5</v>
       </c>
       <c r="B44" s="2">
-        <v>0.4120196104049683</v>
+        <v>0.393620640039444</v>
       </c>
       <c r="C44" s="1">
         <v>58</v>
@@ -2907,7 +2907,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="2">
-        <v>0.3836044669151306</v>
+        <v>0.3664743900299072</v>
       </c>
       <c r="C45" s="1">
         <v>54</v>
@@ -2933,7 +2933,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="2">
-        <v>0.355189323425293</v>
+        <v>0.3393281400203705</v>
       </c>
       <c r="C46" s="1">
         <v>50</v>
@@ -2959,7 +2959,7 @@
         <v>9</v>
       </c>
       <c r="B47" s="2">
-        <v>0.3267741799354553</v>
+        <v>0.3121818900108337</v>
       </c>
       <c r="C47" s="1">
         <v>46</v>
@@ -2985,7 +2985,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2">
-        <v>0.2557363212108612</v>
+        <v>0.2443162500858307</v>
       </c>
       <c r="C48" s="1">
         <v>36</v>
@@ -3011,7 +3011,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2">
-        <v>0.2273211628198624</v>
+        <v>0.217170000076294</v>
       </c>
       <c r="C49" s="1">
         <v>32</v>
@@ -3037,7 +3037,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2">
-        <v>0.1989060193300247</v>
+        <v>0.1900237500667572</v>
       </c>
       <c r="C50" s="1">
         <v>28</v>
@@ -3063,7 +3063,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="2">
-        <v>0.1989060193300247</v>
+        <v>0.1900237500667572</v>
       </c>
       <c r="C51" s="1">
         <v>28</v>
@@ -3089,7 +3089,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2">
-        <v>0.1846984475851059</v>
+        <v>0.1764506250619888</v>
       </c>
       <c r="C52" s="1">
         <v>26</v>
@@ -3115,7 +3115,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>0.1846984475851059</v>
+        <v>0.1764506250619888</v>
       </c>
       <c r="C53" s="1">
         <v>26</v>
@@ -3141,7 +3141,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>0.1846984475851059</v>
+        <v>0.1764506250619888</v>
       </c>
       <c r="C54" s="1">
         <v>26</v>
@@ -3167,7 +3167,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="2">
-        <v>0.1278681606054306</v>
+        <v>0.1221581250429153</v>
       </c>
       <c r="C55" s="1">
         <v>18</v>
@@ -3193,7 +3193,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="2">
-        <v>0.1136605814099312</v>
+        <v>0.108585000038147</v>
       </c>
       <c r="C56" s="1">
         <v>16</v>
@@ -3219,7 +3219,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="2">
-        <v>0.08524543792009354</v>
+        <v>0.08143875002861023</v>
       </c>
       <c r="C57" s="1">
         <v>12</v>
@@ -3245,7 +3245,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>0.08524543792009354</v>
+        <v>0.08143875002861023</v>
       </c>
       <c r="C58" s="1">
         <v>12</v>
@@ -3271,7 +3271,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="2">
-        <v>0.08524543792009354</v>
+        <v>0.08143875002861023</v>
       </c>
       <c r="C59" s="1">
         <v>12</v>
@@ -3297,7 +3297,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>0.07103786617517471</v>
+        <v>0.06786562502384186</v>
       </c>
       <c r="C60" s="1">
         <v>10</v>
@@ -3323,7 +3323,7 @@
         <v>7</v>
       </c>
       <c r="B61" s="2">
-        <v>0.05683029070496559</v>
+        <v>0.05429250001907349</v>
       </c>
       <c r="C61" s="1">
         <v>8</v>
@@ -3349,7 +3349,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="2">
-        <v>0.05683029070496559</v>
+        <v>0.05429250001907349</v>
       </c>
       <c r="C62" s="1">
         <v>8</v>
@@ -3375,7 +3375,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="2">
-        <v>0.04262271896004677</v>
+        <v>0.04071937501430512</v>
       </c>
       <c r="C63" s="1">
         <v>6</v>
@@ -3401,7 +3401,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="2">
-        <v>0.04262271896004677</v>
+        <v>0.04071937501430512</v>
       </c>
       <c r="C64" s="1">
         <v>6</v>
@@ -3427,7 +3427,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="2">
-        <v>0.04262271896004677</v>
+        <v>0.04071937501430512</v>
       </c>
       <c r="C65" s="1">
         <v>6</v>
@@ -3453,7 +3453,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="2">
-        <v>0.0142075726762414</v>
+        <v>0.01357312500476837</v>
       </c>
       <c r="C66" s="1">
         <v>2</v>
@@ -3479,7 +3479,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="2">
-        <v>0.0142075726762414</v>
+        <v>0.01357312500476837</v>
       </c>
       <c r="C67" s="1">
         <v>2</v>
@@ -3505,7 +3505,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="2">
-        <v>0.0142075726762414</v>
+        <v>0.01357312500476837</v>
       </c>
       <c r="C68" s="1">
         <v>2</v>
@@ -3531,7 +3531,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="2">
-        <v>0.0142075726762414</v>
+        <v>0.01357312500476837</v>
       </c>
       <c r="C69" s="1">
         <v>2</v>
@@ -3557,7 +3557,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="2">
-        <v>0.0142075726762414</v>
+        <v>0.01357312500476837</v>
       </c>
       <c r="C70" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
Add RX8900 alarm function
</commit_message>
<xml_diff>
--- a/Software/MDK-ARM/Software_analysis.xlsx
+++ b/Software/MDK-ARM/Software_analysis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="81">
   <si>
     <t>Software</t>
   </si>
@@ -47,12 +47,12 @@
     <t>tx_initialize_high_level.o</t>
   </si>
   <si>
+    <t>rx8900.o</t>
+  </si>
+  <si>
     <t>stm32l4xx_hal.o</t>
   </si>
   <si>
-    <t>rx8900.o</t>
-  </si>
-  <si>
     <t>tx_low_power.o</t>
   </si>
   <si>
@@ -74,24 +74,24 @@
     <t>txe_thread_create.o</t>
   </si>
   <si>
+    <t>tx_thread_system_suspend.o</t>
+  </si>
+  <si>
+    <t>txe_byte_pool_create.o</t>
+  </si>
+  <si>
+    <t>tx_timer_thread_entry.o</t>
+  </si>
+  <si>
+    <t>tx_thread_create.o</t>
+  </si>
+  <si>
+    <t>tx_thread_system_resume.o</t>
+  </si>
+  <si>
     <t>stm32l4xx_hal_pwr_ex.o</t>
   </si>
   <si>
-    <t>tx_thread_system_suspend.o</t>
-  </si>
-  <si>
-    <t>txe_byte_pool_create.o</t>
-  </si>
-  <si>
-    <t>tx_timer_thread_entry.o</t>
-  </si>
-  <si>
-    <t>tx_thread_create.o</t>
-  </si>
-  <si>
-    <t>tx_thread_system_resume.o</t>
-  </si>
-  <si>
     <t>tx_thread_schedule.o</t>
   </si>
   <si>
@@ -107,6 +107,9 @@
     <t>main.o</t>
   </si>
   <si>
+    <t>tx_thread_sleep.o</t>
+  </si>
+  <si>
     <t>stm32l4xx_hal_i2c_ex.o</t>
   </si>
   <si>
@@ -128,19 +131,19 @@
     <t>tx_thread_shell_entry.o</t>
   </si>
   <si>
+    <t>rx8900_callout.o</t>
+  </si>
+  <si>
+    <t>rt_memclr_w.o</t>
+  </si>
+  <si>
+    <t>tx_initialize_kernel_enter.o</t>
+  </si>
+  <si>
+    <t>sys_stackheap_outer.o</t>
+  </si>
+  <si>
     <t>stm32l4xx_hal_pwr.o</t>
-  </si>
-  <si>
-    <t>rx8900_callout.o</t>
-  </si>
-  <si>
-    <t>rt_memclr_w.o</t>
-  </si>
-  <si>
-    <t>tx_initialize_kernel_enter.o</t>
-  </si>
-  <si>
-    <t>sys_stackheap_outer.o</t>
   </si>
   <si>
     <t>rt_memclr.o</t>
@@ -344,9 +347,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ram_percent!$A$3:$A$72</c:f>
+              <c:f>ram_percent!$A$3:$A$73</c:f>
               <c:strCache>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>startup_stm32l432xx.o</c:v>
                 </c:pt>
@@ -375,10 +378,10 @@
                   <c:v>tx_initialize_high_level.o</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>rx8900.o</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>stm32l4xx_hal.o</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>rx8900.o</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>tx_low_power.o</c:v>
@@ -386,7 +389,7 @@
                 <c:pt idx="12">
                   <c:v>system_stm32l4xx.o</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -394,50 +397,50 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ram_percent!$B$3:$B$72</c:f>
+              <c:f>ram_percent!$B$3:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>32.70868682861328</c:v>
+                  <c:v>32.54237365722656</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.55366325378418</c:v>
+                  <c:v>25.48728752136231</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.48381614685059</c:v>
+                  <c:v>18.38982963562012</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.01022148132324</c:v>
+                  <c:v>11.94915294647217</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.662691593170166</c:v>
+                  <c:v>3.644067764282227</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.04429292678833</c:v>
+                  <c:v>2.03389835357666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.04429292678833</c:v>
+                  <c:v>2.03389835357666</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.788756370544434</c:v>
+                  <c:v>1.779661059379578</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.107325434684753</c:v>
+                  <c:v>1.101694941520691</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2555366158485413</c:v>
+                  <c:v>0.6144067645072937</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1703577488660812</c:v>
+                  <c:v>0.2542372941970825</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08517887443304062</c:v>
+                  <c:v>0.08474576473236084</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.08517887443304062</c:v>
-                </c:pt>
-                <c:pt idx="69">
+                  <c:v>0.08474576473236084</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -505,9 +508,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>flash_percent!$A$3:$A$72</c:f>
+              <c:f>flash_percent!$A$3:$A$73</c:f>
               <c:strCache>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>stm32l4xx_hal_rcc.o</c:v>
                 </c:pt>
@@ -536,22 +539,22 @@
                   <c:v>txe_thread_create.o</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>tx_thread_system_suspend.o</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>txe_byte_pool_create.o</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>tx_timer_thread_entry.o</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>tx_thread_create.o</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>tx_thread_system_resume.o</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>stm32l4xx_hal_pwr_ex.o</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>tx_thread_system_suspend.o</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>txe_byte_pool_create.o</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>tx_timer_thread_entry.o</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>tx_thread_create.o</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>tx_thread_system_resume.o</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>i2c.o</c:v>
@@ -566,10 +569,10 @@
                   <c:v>tx_timer_interrupt.o</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>stm32l4xx_hal.o</c:v>
+                  <c:v>tx_timer_initialize.o</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>tx_timer_initialize.o</c:v>
+                  <c:v>appmain.o</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>tx_initialize_low_level.o</c:v>
@@ -578,31 +581,31 @@
                   <c:v>main.o</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>tx_thread_sleep.o</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>stm32l4xx_hal_i2c_ex.o</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>tx_byte_pool_create.o</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>appmain.o</c:v>
-                </c:pt>
                 <c:pt idx="26">
+                  <c:v>stm32l4xx_hal.o</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>tx_thread_time_slice.o</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>gpio.o</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>__scatter.o</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>tx_timer_system_activate.o</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>tx_thread_shell_entry.o</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>stm32l4xx_hal_pwr.o</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>rx8900_callout.o</c:v>
@@ -623,99 +626,102 @@
                   <c:v>sys_stackheap_outer.o</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>stm32l4xx_hal_pwr.o</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>rt_memclr.o</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>tx_thread_stack_build.o</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>tx_timer_system_deactivate.o</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>tx_thread_initialize.o</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>tx_thread_timeout.o</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>stm32l4xx_hal_msp.o</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>tx_initialize_high_level.o</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>tx_timer_expiration_process.o</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>__scatter_zi.o</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>app_threadx.o</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>fz_wm.l</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>fpinit.o</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>__scatter_copy.o</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>exit.o</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>stm32l4xx_it.o</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>aeabi_memset.o</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>sys_exit.o</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>__rtentry2.o</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>rtexit2.o</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>appirqcallout.o</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>libspace.o</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>__main.o</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>libinit2.o</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>heapauxi.o</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>__rtentry4.o</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>rx8900_lcfg.o</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>use_no_semi.o</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>rtexit.o</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>libshutdown2.o</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>libshutdown.o</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>libinit.o</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -723,218 +729,221 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flash_percent!$B$3:$B$72</c:f>
+              <c:f>flash_percent!$B$3:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>17.51776695251465</c:v>
+                  <c:v>16.9673023223877</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.12213706970215</c:v>
+                  <c:v>13.67837333679199</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.7386155128479</c:v>
+                  <c:v>9.656447410583496</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.409581661224365</c:v>
+                  <c:v>6.208171367645264</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.554093360900879</c:v>
+                  <c:v>5.379565238952637</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.15872597694397</c:v>
+                  <c:v>3.059468507766724</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.040273666381836</c:v>
+                  <c:v>2.944738388061523</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.027112483978272</c:v>
+                  <c:v>2.931990623474121</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.619110345840454</c:v>
+                  <c:v>2.536809206008911</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.566464900970459</c:v>
+                  <c:v>2.422079086303711</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.50065803527832</c:v>
+                  <c:v>2.269105672836304</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.342721700668335</c:v>
+                  <c:v>2.07788896560669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.145301342010498</c:v>
+                  <c:v>2.02689790725708</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.092655897140503</c:v>
+                  <c:v>1.963158845901489</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.026849269866943</c:v>
+                  <c:v>1.759194374084473</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.592524290084839</c:v>
+                  <c:v>1.542482018470764</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.447749376296997</c:v>
+                  <c:v>1.402256369590759</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.289813160896301</c:v>
+                  <c:v>1.249282956123352</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.210844993591309</c:v>
+                  <c:v>1.172796249389648</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.066069960594177</c:v>
+                  <c:v>1.019822835922241</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.052908658981323</c:v>
+                  <c:v>1.019822835922241</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.000263214111328</c:v>
+                  <c:v>0.9688316583633423</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.9739404916763306</c:v>
+                  <c:v>0.9433360695838928</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.9607791304588318</c:v>
+                  <c:v>0.9305883049964905</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.9212951064109802</c:v>
+                  <c:v>0.9305883049964905</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.9081337451934815</c:v>
+                  <c:v>0.8923449516296387</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.7370360493659973</c:v>
+                  <c:v>0.8031104803085327</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.6712292432785034</c:v>
+                  <c:v>0.713875949382782</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.6185838580131531</c:v>
+                  <c:v>0.6501370668411255</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.5922611355781555</c:v>
+                  <c:v>0.5991458892822266</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.5922611355781555</c:v>
+                  <c:v>0.5736503005027771</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.5922611355781555</c:v>
+                  <c:v>0.5736503005027771</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.5922611355781555</c:v>
+                  <c:v>0.5736503005027771</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.565938413143158</c:v>
+                  <c:v>0.5481547713279724</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.5527770519256592</c:v>
+                  <c:v>0.5354069471359253</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.5132929682731628</c:v>
+                  <c:v>0.4971636235713959</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.5132929682731628</c:v>
+                  <c:v>0.4971636235713959</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.4869702458381653</c:v>
+                  <c:v>0.4716680347919464</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.4474861919879913</c:v>
+                  <c:v>0.4716680347919464</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.4211634695529938</c:v>
+                  <c:v>0.4334246814250946</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.3816793859004974</c:v>
+                  <c:v>0.4079291224479675</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.3816793859004974</c:v>
+                  <c:v>0.3696857690811157</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.3553566634654999</c:v>
+                  <c:v>0.3696857690811157</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.3290339708328247</c:v>
+                  <c:v>0.3441902101039887</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.3027112483978272</c:v>
+                  <c:v>0.3186946213245392</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.2369044423103333</c:v>
+                  <c:v>0.2931990623474121</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.1842590123414993</c:v>
+                  <c:v>0.229460135102272</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.1842590123414993</c:v>
+                  <c:v>0.1784689873456955</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.1710976511240006</c:v>
+                  <c:v>0.1784689873456955</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.1710976511240006</c:v>
+                  <c:v>0.165721207857132</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.1710976511240006</c:v>
+                  <c:v>0.165721207857132</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.1184522211551666</c:v>
+                  <c:v>0.165721207857132</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.1184522211551666</c:v>
+                  <c:v>0.114730067551136</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.1052908673882484</c:v>
+                  <c:v>0.114730067551136</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.07896815240383148</c:v>
+                  <c:v>0.1019822806119919</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.07896815240383148</c:v>
+                  <c:v>0.07648670673370361</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.0658067911863327</c:v>
+                  <c:v>0.07648670673370361</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.0658067911863327</c:v>
+                  <c:v>0.06373892724514008</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.05264543369412422</c:v>
+                  <c:v>0.06373892724514008</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.05264543369412422</c:v>
+                  <c:v>0.05099114030599594</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.03948407620191574</c:v>
+                  <c:v>0.05099114030599594</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.03948407620191574</c:v>
+                  <c:v>0.03824335336685181</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.03948407620191574</c:v>
+                  <c:v>0.03824335336685181</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.02632271684706211</c:v>
+                  <c:v>0.03824335336685181</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.01316135842353106</c:v>
+                  <c:v>0.02549557015299797</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.01316135842353106</c:v>
+                  <c:v>0.01274778507649899</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.01316135842353106</c:v>
+                  <c:v>0.01274778507649899</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.01316135842353106</c:v>
+                  <c:v>0.01274778507649899</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.01316135842353106</c:v>
+                  <c:v>0.01274778507649899</c:v>
                 </c:pt>
                 <c:pt idx="69">
+                  <c:v>0.01274778507649899</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1039,8 +1048,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H72" totalsRowCount="1">
-  <autoFilter ref="A2:H71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H73" totalsRowCount="1">
+  <autoFilter ref="A2:H72"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="ram_percent" totalsRowFunction="sum"/>
@@ -1056,8 +1065,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H72" totalsRowCount="1">
-  <autoFilter ref="A2:H71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H73" totalsRowCount="1">
+  <autoFilter ref="A2:H72"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="flash_percent" totalsRowFunction="sum"/>
@@ -1357,7 +1366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1373,28 +1382,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1402,7 +1411,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>32.70868682861328</v>
+        <v>32.54237365722656</v>
       </c>
       <c r="C3" s="1">
         <v>1536</v>
@@ -1428,16 +1437,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>25.55366325378418</v>
+        <v>25.48728752136231</v>
       </c>
       <c r="C4" s="1">
-        <v>1200</v>
+        <v>1203</v>
       </c>
       <c r="D4" s="1">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="E4" s="1">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1446,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>1200</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1454,7 +1463,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>18.48381614685059</v>
+        <v>18.38982963562012</v>
       </c>
       <c r="C5" s="1">
         <v>868</v>
@@ -1480,7 +1489,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>12.01022148132324</v>
+        <v>11.94915294647217</v>
       </c>
       <c r="C6" s="1">
         <v>564</v>
@@ -1506,7 +1515,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>3.662691593170166</v>
+        <v>3.644067764282227</v>
       </c>
       <c r="C7" s="1">
         <v>172</v>
@@ -1532,7 +1541,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>2.04429292678833</v>
+        <v>2.03389835357666</v>
       </c>
       <c r="C8" s="1">
         <v>96</v>
@@ -1558,7 +1567,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>2.04429292678833</v>
+        <v>2.03389835357666</v>
       </c>
       <c r="C9" s="1">
         <v>96</v>
@@ -1584,7 +1593,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>1.788756370544434</v>
+        <v>1.779661059379578</v>
       </c>
       <c r="C10" s="1">
         <v>84</v>
@@ -1610,7 +1619,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>1.107325434684753</v>
+        <v>1.101694941520691</v>
       </c>
       <c r="C11" s="1">
         <v>52</v>
@@ -1636,25 +1645,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>0.2555366158485413</v>
+        <v>0.6144067645072937</v>
       </c>
       <c r="C12" s="1">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1">
-        <v>162</v>
+        <v>1515</v>
       </c>
       <c r="E12" s="1">
-        <v>154</v>
+        <v>1514</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1662,25 +1671,25 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>0.1703577488660812</v>
+        <v>0.2542372941970825</v>
       </c>
       <c r="C13" s="1">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1">
+        <v>126</v>
+      </c>
+      <c r="E13" s="1">
+        <v>118</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
         <v>8</v>
       </c>
-      <c r="D13" s="1">
-        <v>1024</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1024</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
       <c r="H13" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1688,7 +1697,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>0.08517887443304062</v>
+        <v>0.08474576473236084</v>
       </c>
       <c r="C14" s="1">
         <v>4</v>
@@ -1714,7 +1723,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>0.08517887443304062</v>
+        <v>0.08474576473236084</v>
       </c>
       <c r="C15" s="1">
         <v>4</v>
@@ -1735,35 +1744,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
-      <c r="A72" t="s">
-        <v>71</v>
-      </c>
-      <c r="B72">
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73">
         <f>SUBTOTAL(109,[ram_percent])</f>
         <v>0</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="D72">
+      <c r="D73">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="E72">
+      <c r="E73">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F72">
+      <c r="F73">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G72">
+      <c r="G73">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H72">
+      <c r="H73">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>
@@ -1779,7 +1788,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1795,28 +1804,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
         <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1824,7 +1833,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="2">
-        <v>17.51776695251465</v>
+        <v>16.9673023223877</v>
       </c>
       <c r="C3" s="1">
         <v>2662</v>
@@ -1850,7 +1859,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="2">
-        <v>14.12213706970215</v>
+        <v>13.67837333679199</v>
       </c>
       <c r="C4" s="1">
         <v>2146</v>
@@ -1873,28 +1882,28 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
-        <v>6.7386155128479</v>
+        <v>9.656447410583496</v>
       </c>
       <c r="C5" s="1">
-        <v>1024</v>
+        <v>1515</v>
       </c>
       <c r="D5" s="1">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1">
-        <v>1024</v>
+        <v>1514</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1902,7 +1911,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="2">
-        <v>6.409581661224365</v>
+        <v>6.208171367645264</v>
       </c>
       <c r="C6" s="1">
         <v>974</v>
@@ -1928,7 +1937,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2">
-        <v>5.554093360900879</v>
+        <v>5.379565238952637</v>
       </c>
       <c r="C7" s="1">
         <v>844</v>
@@ -1954,7 +1963,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>3.15872597694397</v>
+        <v>3.059468507766724</v>
       </c>
       <c r="C8" s="1">
         <v>480</v>
@@ -1980,7 +1989,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2">
-        <v>3.040273666381836</v>
+        <v>2.944738388061523</v>
       </c>
       <c r="C9" s="1">
         <v>462</v>
@@ -2006,7 +2015,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="2">
-        <v>3.027112483978272</v>
+        <v>2.931990623474121</v>
       </c>
       <c r="C10" s="1">
         <v>460</v>
@@ -2032,7 +2041,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="2">
-        <v>2.619110345840454</v>
+        <v>2.536809206008911</v>
       </c>
       <c r="C11" s="1">
         <v>398</v>
@@ -2058,16 +2067,16 @@
         <v>19</v>
       </c>
       <c r="B12" s="2">
-        <v>2.566464900970459</v>
+        <v>2.422079086303711</v>
       </c>
       <c r="C12" s="1">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -2084,16 +2093,16 @@
         <v>20</v>
       </c>
       <c r="B13" s="2">
-        <v>2.50065803527832</v>
+        <v>2.269105672836304</v>
       </c>
       <c r="C13" s="1">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -2110,16 +2119,16 @@
         <v>21</v>
       </c>
       <c r="B14" s="2">
-        <v>2.342721700668335</v>
+        <v>2.07788896560669</v>
       </c>
       <c r="C14" s="1">
-        <v>356</v>
+        <v>326</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>356</v>
+        <v>326</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -2136,16 +2145,16 @@
         <v>22</v>
       </c>
       <c r="B15" s="2">
-        <v>2.145301342010498</v>
+        <v>2.02689790725708</v>
       </c>
       <c r="C15" s="1">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -2162,16 +2171,16 @@
         <v>23</v>
       </c>
       <c r="B16" s="2">
-        <v>2.092655897140503</v>
+        <v>1.963158845901489</v>
       </c>
       <c r="C16" s="1">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -2188,16 +2197,16 @@
         <v>24</v>
       </c>
       <c r="B17" s="2">
-        <v>2.026849269866943</v>
+        <v>1.759194374084473</v>
       </c>
       <c r="C17" s="1">
-        <v>308</v>
+        <v>276</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>308</v>
+        <v>276</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -2214,7 +2223,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="2">
-        <v>1.592524290084839</v>
+        <v>1.542482018470764</v>
       </c>
       <c r="C18" s="1">
         <v>242</v>
@@ -2240,7 +2249,7 @@
         <v>25</v>
       </c>
       <c r="B19" s="2">
-        <v>1.447749376296997</v>
+        <v>1.402256369590759</v>
       </c>
       <c r="C19" s="1">
         <v>220</v>
@@ -2266,7 +2275,7 @@
         <v>26</v>
       </c>
       <c r="B20" s="2">
-        <v>1.289813160896301</v>
+        <v>1.249282956123352</v>
       </c>
       <c r="C20" s="1">
         <v>196</v>
@@ -2292,7 +2301,7 @@
         <v>27</v>
       </c>
       <c r="B21" s="2">
-        <v>1.210844993591309</v>
+        <v>1.172796249389648</v>
       </c>
       <c r="C21" s="1">
         <v>184</v>
@@ -2315,42 +2324,42 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B22" s="2">
-        <v>1.066069960594177</v>
+        <v>1.019822835922241</v>
       </c>
       <c r="C22" s="1">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D22" s="1">
-        <v>12</v>
+        <v>868</v>
       </c>
       <c r="E22" s="1">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
       </c>
       <c r="G22" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>4</v>
+        <v>868</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23" s="2">
-        <v>1.052908658981323</v>
+        <v>1.019822835922241</v>
       </c>
       <c r="C23" s="1">
         <v>160</v>
       </c>
       <c r="D23" s="1">
-        <v>868</v>
+        <v>1203</v>
       </c>
       <c r="E23" s="1">
         <v>160</v>
@@ -2362,7 +2371,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>868</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2370,7 +2379,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="2">
-        <v>1.000263214111328</v>
+        <v>0.9688316583633423</v>
       </c>
       <c r="C24" s="1">
         <v>152</v>
@@ -2396,7 +2405,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="2">
-        <v>0.9739404916763306</v>
+        <v>0.9433360695838928</v>
       </c>
       <c r="C25" s="1">
         <v>148</v>
@@ -2422,7 +2431,7 @@
         <v>30</v>
       </c>
       <c r="B26" s="2">
-        <v>0.9607791304588318</v>
+        <v>0.9305883049964905</v>
       </c>
       <c r="C26" s="1">
         <v>146</v>
@@ -2448,16 +2457,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="2">
-        <v>0.9212951064109802</v>
+        <v>0.9305883049964905</v>
       </c>
       <c r="C27" s="1">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -2471,19 +2480,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2">
-        <v>0.9081337451934815</v>
+        <v>0.8923449516296387</v>
       </c>
       <c r="C28" s="1">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D28" s="1">
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -2492,33 +2501,33 @@
         <v>0</v>
       </c>
       <c r="H28" s="1">
-        <v>1200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B29" s="2">
-        <v>0.7370360493659973</v>
+        <v>0.8031104803085327</v>
       </c>
       <c r="C29" s="1">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E29" s="1">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
       </c>
       <c r="G29" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H29" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2526,16 +2535,16 @@
         <v>33</v>
       </c>
       <c r="B30" s="2">
-        <v>0.6712292432785034</v>
+        <v>0.713875949382782</v>
       </c>
       <c r="C30" s="1">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -2552,16 +2561,16 @@
         <v>34</v>
       </c>
       <c r="B31" s="2">
-        <v>0.6185838580131531</v>
+        <v>0.6501370668411255</v>
       </c>
       <c r="C31" s="1">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -2578,16 +2587,16 @@
         <v>35</v>
       </c>
       <c r="B32" s="2">
-        <v>0.5922611355781555</v>
+        <v>0.5991458892822266</v>
       </c>
       <c r="C32" s="1">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -2604,7 +2613,7 @@
         <v>36</v>
       </c>
       <c r="B33" s="2">
-        <v>0.5922611355781555</v>
+        <v>0.5736503005027771</v>
       </c>
       <c r="C33" s="1">
         <v>90</v>
@@ -2630,7 +2639,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="2">
-        <v>0.5922611355781555</v>
+        <v>0.5736503005027771</v>
       </c>
       <c r="C34" s="1">
         <v>90</v>
@@ -2656,7 +2665,7 @@
         <v>38</v>
       </c>
       <c r="B35" s="2">
-        <v>0.5922611355781555</v>
+        <v>0.5736503005027771</v>
       </c>
       <c r="C35" s="1">
         <v>90</v>
@@ -2682,7 +2691,7 @@
         <v>13</v>
       </c>
       <c r="B36" s="2">
-        <v>0.565938413143158</v>
+        <v>0.5481547713279724</v>
       </c>
       <c r="C36" s="1">
         <v>86</v>
@@ -2708,7 +2717,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="2">
-        <v>0.5527770519256592</v>
+        <v>0.5354069471359253</v>
       </c>
       <c r="C37" s="1">
         <v>84</v>
@@ -2734,7 +2743,7 @@
         <v>39</v>
       </c>
       <c r="B38" s="2">
-        <v>0.5132929682731628</v>
+        <v>0.4971636235713959</v>
       </c>
       <c r="C38" s="1">
         <v>78</v>
@@ -2760,7 +2769,7 @@
         <v>40</v>
       </c>
       <c r="B39" s="2">
-        <v>0.5132929682731628</v>
+        <v>0.4971636235713959</v>
       </c>
       <c r="C39" s="1">
         <v>78</v>
@@ -2786,7 +2795,7 @@
         <v>41</v>
       </c>
       <c r="B40" s="2">
-        <v>0.4869702458381653</v>
+        <v>0.4716680347919464</v>
       </c>
       <c r="C40" s="1">
         <v>74</v>
@@ -2812,16 +2821,16 @@
         <v>42</v>
       </c>
       <c r="B41" s="2">
-        <v>0.4474861919879913</v>
+        <v>0.4716680347919464</v>
       </c>
       <c r="C41" s="1">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
@@ -2838,16 +2847,16 @@
         <v>43</v>
       </c>
       <c r="B42" s="2">
-        <v>0.4211634695529938</v>
+        <v>0.4334246814250946</v>
       </c>
       <c r="C42" s="1">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F42" s="1">
         <v>0</v>
@@ -2864,16 +2873,16 @@
         <v>44</v>
       </c>
       <c r="B43" s="2">
-        <v>0.3816793859004974</v>
+        <v>0.4079291224479675</v>
       </c>
       <c r="C43" s="1">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
       </c>
       <c r="E43" s="1">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F43" s="1">
         <v>0</v>
@@ -2887,42 +2896,42 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B44" s="2">
-        <v>0.3816793859004974</v>
+        <v>0.3696857690811157</v>
       </c>
       <c r="C44" s="1">
         <v>58</v>
       </c>
       <c r="D44" s="1">
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="E44" s="1">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F44" s="1">
         <v>0</v>
       </c>
       <c r="G44" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H44" s="1">
-        <v>168</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B45" s="2">
-        <v>0.3553566634654999</v>
+        <v>0.3696857690811157</v>
       </c>
       <c r="C45" s="1">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D45" s="1">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="E45" s="1">
         <v>54</v>
@@ -2931,10 +2940,10 @@
         <v>0</v>
       </c>
       <c r="G45" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H45" s="1">
-        <v>0</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2942,16 +2951,16 @@
         <v>46</v>
       </c>
       <c r="B46" s="2">
-        <v>0.3290339708328247</v>
+        <v>0.3441902101039887</v>
       </c>
       <c r="C46" s="1">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
       </c>
       <c r="E46" s="1">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F46" s="1">
         <v>0</v>
@@ -2965,19 +2974,19 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B47" s="2">
-        <v>0.3027112483978272</v>
+        <v>0.3186946213245392</v>
       </c>
       <c r="C47" s="1">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D47" s="1">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E47" s="1">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F47" s="1">
         <v>0</v>
@@ -2986,24 +2995,24 @@
         <v>0</v>
       </c>
       <c r="H47" s="1">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B48" s="2">
-        <v>0.2369044423103333</v>
+        <v>0.2931990623474121</v>
       </c>
       <c r="C48" s="1">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D48" s="1">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E48" s="1">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F48" s="1">
         <v>0</v>
@@ -3012,7 +3021,7 @@
         <v>0</v>
       </c>
       <c r="H48" s="1">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3020,16 +3029,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="2">
-        <v>0.1842590123414993</v>
+        <v>0.229460135102272</v>
       </c>
       <c r="C49" s="1">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
       </c>
       <c r="E49" s="1">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F49" s="1">
         <v>0</v>
@@ -3046,7 +3055,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2">
-        <v>0.1842590123414993</v>
+        <v>0.1784689873456955</v>
       </c>
       <c r="C50" s="1">
         <v>28</v>
@@ -3072,16 +3081,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="2">
-        <v>0.1710976511240006</v>
+        <v>0.1784689873456955</v>
       </c>
       <c r="C51" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
       </c>
       <c r="E51" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
@@ -3098,7 +3107,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2">
-        <v>0.1710976511240006</v>
+        <v>0.165721207857132</v>
       </c>
       <c r="C52" s="1">
         <v>26</v>
@@ -3124,7 +3133,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>0.1710976511240006</v>
+        <v>0.165721207857132</v>
       </c>
       <c r="C53" s="1">
         <v>26</v>
@@ -3150,16 +3159,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>0.1184522211551666</v>
+        <v>0.165721207857132</v>
       </c>
       <c r="C54" s="1">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D54" s="1">
         <v>0</v>
       </c>
       <c r="E54" s="1">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F54" s="1">
         <v>0</v>
@@ -3176,7 +3185,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="2">
-        <v>0.1184522211551666</v>
+        <v>0.114730067551136</v>
       </c>
       <c r="C55" s="1">
         <v>18</v>
@@ -3202,16 +3211,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="2">
-        <v>0.1052908673882484</v>
+        <v>0.114730067551136</v>
       </c>
       <c r="C56" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
       </c>
       <c r="E56" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
@@ -3228,16 +3237,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="2">
-        <v>0.07896815240383148</v>
+        <v>0.1019822806119919</v>
       </c>
       <c r="C57" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
       </c>
       <c r="E57" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
@@ -3254,7 +3263,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>0.07896815240383148</v>
+        <v>0.07648670673370361</v>
       </c>
       <c r="C58" s="1">
         <v>12</v>
@@ -3280,16 +3289,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="2">
-        <v>0.0658067911863327</v>
+        <v>0.07648670673370361</v>
       </c>
       <c r="C59" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
       </c>
       <c r="E59" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F59" s="1">
         <v>0</v>
@@ -3306,7 +3315,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>0.0658067911863327</v>
+        <v>0.06373892724514008</v>
       </c>
       <c r="C60" s="1">
         <v>10</v>
@@ -3329,19 +3338,19 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="B61" s="2">
-        <v>0.05264543369412422</v>
+        <v>0.06373892724514008</v>
       </c>
       <c r="C61" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D61" s="1">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="E61" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F61" s="1">
         <v>0</v>
@@ -3350,21 +3359,21 @@
         <v>0</v>
       </c>
       <c r="H61" s="1">
-        <v>96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="B62" s="2">
-        <v>0.05264543369412422</v>
+        <v>0.05099114030599594</v>
       </c>
       <c r="C62" s="1">
         <v>8</v>
       </c>
       <c r="D62" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="E62" s="1">
         <v>8</v>
@@ -3376,7 +3385,7 @@
         <v>0</v>
       </c>
       <c r="H62" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -3384,16 +3393,16 @@
         <v>61</v>
       </c>
       <c r="B63" s="2">
-        <v>0.03948407620191574</v>
+        <v>0.05099114030599594</v>
       </c>
       <c r="C63" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D63" s="1">
         <v>0</v>
       </c>
       <c r="E63" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F63" s="1">
         <v>0</v>
@@ -3410,7 +3419,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="2">
-        <v>0.03948407620191574</v>
+        <v>0.03824335336685181</v>
       </c>
       <c r="C64" s="1">
         <v>6</v>
@@ -3436,7 +3445,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="2">
-        <v>0.03948407620191574</v>
+        <v>0.03824335336685181</v>
       </c>
       <c r="C65" s="1">
         <v>6</v>
@@ -3462,19 +3471,19 @@
         <v>64</v>
       </c>
       <c r="B66" s="2">
-        <v>0.02632271684706211</v>
+        <v>0.03824335336685181</v>
       </c>
       <c r="C66" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D66" s="1">
         <v>0</v>
       </c>
       <c r="E66" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F66" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G66" s="1">
         <v>0</v>
@@ -3488,19 +3497,19 @@
         <v>65</v>
       </c>
       <c r="B67" s="2">
-        <v>0.01316135842353106</v>
+        <v>0.02549557015299797</v>
       </c>
       <c r="C67" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D67" s="1">
         <v>0</v>
       </c>
       <c r="E67" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F67" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G67" s="1">
         <v>0</v>
@@ -3514,7 +3523,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="2">
-        <v>0.01316135842353106</v>
+        <v>0.01274778507649899</v>
       </c>
       <c r="C68" s="1">
         <v>2</v>
@@ -3540,7 +3549,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="2">
-        <v>0.01316135842353106</v>
+        <v>0.01274778507649899</v>
       </c>
       <c r="C69" s="1">
         <v>2</v>
@@ -3566,7 +3575,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="2">
-        <v>0.01316135842353106</v>
+        <v>0.01274778507649899</v>
       </c>
       <c r="C70" s="1">
         <v>2</v>
@@ -3592,7 +3601,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="2">
-        <v>0.01316135842353106</v>
+        <v>0.01274778507649899</v>
       </c>
       <c r="C71" s="1">
         <v>2</v>
@@ -3614,34 +3623,60 @@
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" t="s">
-        <v>71</v>
-      </c>
-      <c r="B72">
+      <c r="A72" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" s="2">
+        <v>0.01274778507649899</v>
+      </c>
+      <c r="C72" s="1">
+        <v>2</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0</v>
+      </c>
+      <c r="E72" s="1">
+        <v>2</v>
+      </c>
+      <c r="F72" s="1">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1">
+        <v>0</v>
+      </c>
+      <c r="H72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73">
         <f>SUBTOTAL(109,[flash_percent])</f>
         <v>0</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="D72">
+      <c r="D73">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="E72">
+      <c r="E73">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F72">
+      <c r="F73">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G72">
+      <c r="G73">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H72">
+      <c r="H73">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
完善add lptim low power sleep
</commit_message>
<xml_diff>
--- a/Software/MDK-ARM/Software_analysis.xlsx
+++ b/Software/MDK-ARM/Software_analysis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="89">
   <si>
     <t>Software</t>
   </si>
@@ -44,12 +44,18 @@
     <t>i2c.o</t>
   </si>
   <si>
+    <t>lptim.o</t>
+  </si>
+  <si>
     <t>tx_initialize_high_level.o</t>
   </si>
   <si>
     <t>applowpowermgr.o</t>
   </si>
   <si>
+    <t>stm32l4xx_hal.o</t>
+  </si>
+  <si>
     <t>rx8900.o</t>
   </si>
   <si>
@@ -59,7 +65,7 @@
     <t>system_stm32l4xx.o</t>
   </si>
   <si>
-    <t>stm32l4xx_hal.o</t>
+    <t>appirqcallout.o</t>
   </si>
   <si>
     <t>stm32l4xx_hal_rcc.o</t>
@@ -68,34 +74,49 @@
     <t>stm32l4xx_hal_i2c.o</t>
   </si>
   <si>
+    <t>stm32l4xx_hal_lptim.o</t>
+  </si>
+  <si>
     <t>stm32l4xx_hal_rcc_ex.o</t>
   </si>
   <si>
     <t>stm32l4xx_hal_gpio.o</t>
   </si>
   <si>
+    <t>txe_thread_create.o</t>
+  </si>
+  <si>
     <t>tx_thread_system_suspend.o</t>
   </si>
   <si>
-    <t>txe_thread_create.o</t>
+    <t>txe_byte_pool_create.o</t>
+  </si>
+  <si>
+    <t>tx_timer_thread_entry.o</t>
   </si>
   <si>
     <t>tx_thread_create.o</t>
   </si>
   <si>
-    <t>tx_timer_thread_entry.o</t>
+    <t>stm32l4xx_hal_pwr_ex.o</t>
+  </si>
+  <si>
+    <t>tx_thread_schedule.o</t>
   </si>
   <si>
     <t>tx_thread_system_resume.o</t>
   </si>
   <si>
-    <t>stm32l4xx_hal_pwr_ex.o</t>
-  </si>
-  <si>
     <t>stm32l4xx_hal_cortex.o</t>
   </si>
   <si>
-    <t>txe_byte_pool_create.o</t>
+    <t>tx_timer_interrupt.o</t>
+  </si>
+  <si>
+    <t>tx_initialize_low_level.o</t>
+  </si>
+  <si>
+    <t>main.o</t>
   </si>
   <si>
     <t>stm32l4xx_hal_i2c_ex.o</t>
@@ -104,94 +125,82 @@
     <t>tx_byte_pool_create.o</t>
   </si>
   <si>
-    <t>tx_thread_schedule.o</t>
+    <t>gpio.o</t>
   </si>
   <si>
     <t>tx_thread_sleep.o</t>
   </si>
   <si>
+    <t>tx_thread_time_slice.o</t>
+  </si>
+  <si>
+    <t>__scatter.o</t>
+  </si>
+  <si>
     <t>tx_timer_system_activate.o</t>
   </si>
   <si>
-    <t>tx_timer_interrupt.o</t>
-  </si>
-  <si>
-    <t>main.o</t>
-  </si>
-  <si>
-    <t>gpio.o</t>
-  </si>
-  <si>
     <t>rx8900_callout.o</t>
   </si>
   <si>
-    <t>tx_initialize_low_level.o</t>
-  </si>
-  <si>
-    <t>tx_thread_time_slice.o</t>
-  </si>
-  <si>
     <t>tx_thread_shell_entry.o</t>
   </si>
   <si>
+    <t>rt_memclr_w.o</t>
+  </si>
+  <si>
+    <t>tx_initialize_kernel_enter.o</t>
+  </si>
+  <si>
+    <t>sys_stackheap_outer.o</t>
+  </si>
+  <si>
     <t>stm32l4xx_hal_pwr.o</t>
   </si>
   <si>
+    <t>tx_thread_timeout.o</t>
+  </si>
+  <si>
+    <t>rt_memclr.o</t>
+  </si>
+  <si>
+    <t>tx_thread_stack_build.o</t>
+  </si>
+  <si>
     <t>tx_timer_system_deactivate.o</t>
   </si>
   <si>
-    <t>tx_initialize_kernel_enter.o</t>
-  </si>
-  <si>
-    <t>tx_thread_timeout.o</t>
-  </si>
-  <si>
-    <t>__scatter.o</t>
+    <t>stm32l4xx_hal_msp.o</t>
   </si>
   <si>
     <t>app_threadx.o</t>
   </si>
   <si>
-    <t>rt_memclr_w.o</t>
-  </si>
-  <si>
-    <t>sys_stackheap_outer.o</t>
-  </si>
-  <si>
-    <t>rt_memclr.o</t>
-  </si>
-  <si>
-    <t>stm32l4xx_hal_msp.o</t>
-  </si>
-  <si>
-    <t>tx_thread_stack_build.o</t>
-  </si>
-  <si>
     <t>tx_timer_expiration_process.o</t>
   </si>
   <si>
     <t>tx_thread_system_return.o</t>
   </si>
   <si>
+    <t>stm32l4xx_it.o</t>
+  </si>
+  <si>
+    <t>__scatter_zi.o</t>
+  </si>
+  <si>
+    <t>fz_wm.l</t>
+  </si>
+  <si>
+    <t>fpinit.o</t>
+  </si>
+  <si>
+    <t>__scatter_copy.o</t>
+  </si>
+  <si>
+    <t>tx_time_set.o</t>
+  </si>
+  <si>
     <t>tx_time_get.o</t>
-  </si>
-  <si>
-    <t>stm32l4xx_it.o</t>
-  </si>
-  <si>
-    <t>__scatter_zi.o</t>
-  </si>
-  <si>
-    <t>appirqcallout.o</t>
-  </si>
-  <si>
-    <t>fz_wm.l</t>
-  </si>
-  <si>
-    <t>fpinit.o</t>
-  </si>
-  <si>
-    <t>__scatter_copy.o</t>
   </si>
   <si>
     <t>exit.o</t>
@@ -362,9 +371,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ram_percent!$A$3:$A$78</c:f>
+              <c:f>ram_percent!$A$3:$A$81</c:f>
               <c:strCache>
-                <c:ptCount val="76"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>startup_stm32l432xx.o</c:v>
                 </c:pt>
@@ -390,24 +399,30 @@
                   <c:v>i2c.o</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>lptim.o</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>tx_initialize_high_level.o</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>applowpowermgr.o</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
+                  <c:v>stm32l4xx_hal.o</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>rx8900.o</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>tx_low_power.o</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>system_stm32l4xx.o</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>stm32l4xx_hal.o</c:v>
-                </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="15">
+                  <c:v>appirqcallout.o</c:v>
+                </c:pt>
+                <c:pt idx="78">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -415,53 +430,59 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ram_percent!$B$3:$B$78</c:f>
+              <c:f>ram_percent!$B$3:$B$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="76"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
-                  <c:v>32.57688140869141</c:v>
+                  <c:v>32.15407180786133</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.76882362365723</c:v>
+                  <c:v>25.30877113342285</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.40933227539063</c:v>
+                  <c:v>18.17040061950684</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.96182441711426</c:v>
+                  <c:v>11.80657291412354</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.647932052612305</c:v>
+                  <c:v>3.600586175918579</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.036055088043213</c:v>
+                  <c:v>2.009629487991333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.036055088043213</c:v>
+                  <c:v>2.009629487991333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.781548261642456</c:v>
+                  <c:v>1.758425831794739</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.102863192558289</c:v>
+                  <c:v>1.172283887863159</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2545068860054016</c:v>
+                  <c:v>1.088549256324768</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1696712672710419</c:v>
+                  <c:v>0.334938257932663</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08483563363552094</c:v>
+                  <c:v>0.1674691289663315</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.08483563363552094</c:v>
+                  <c:v>0.1674691289663315</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.08483563363552094</c:v>
-                </c:pt>
-                <c:pt idx="75">
+                  <c:v>0.08373456448316574</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.08373456448316574</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.08373456448316574</c:v>
+                </c:pt>
+                <c:pt idx="78">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -529,9 +550,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>flash_percent!$A$3:$A$78</c:f>
+              <c:f>flash_percent!$A$3:$A$81</c:f>
               <c:strCache>
-                <c:ptCount val="76"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>stm32l4xx_hal_rcc.o</c:v>
                 </c:pt>
@@ -539,225 +560,234 @@
                   <c:v>stm32l4xx_hal_i2c.o</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>stm32l4xx_hal_rcc_ex.o</c:v>
+                  <c:v>stm32l4xx_hal_lptim.o</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>rx8900.o</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>stm32l4xx_hal_rcc_ex.o</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tx_low_power.o</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>applowpowermgr.o</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>stm32l4xx_hal_gpio.o</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
+                  <c:v>c_w.l</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>startup_stm32l432xx.o</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>appmain.o</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>txe_thread_create.o</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>tx_thread_system_suspend.o</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>tx_low_power.o</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>txe_thread_create.o</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13">
+                  <c:v>txe_byte_pool_create.o</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>tx_timer_thread_entry.o</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>tx_thread_create.o</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>c_w.l</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>tx_timer_thread_entry.o</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="16">
+                  <c:v>i2c.o</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>stm32l4xx_hal_pwr_ex.o</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>tx_thread_schedule.o</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>tx_thread_system_resume.o</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>startup_stm32l432xx.o</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>stm32l4xx_hal_pwr_ex.o</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="20">
+                  <c:v>lptim.o</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>stm32l4xx_hal_cortex.o</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>appmain.o</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>applowpowermgr.o</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>i2c.o</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>txe_byte_pool_create.o</c:v>
-                </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
+                  <c:v>tx_timer_interrupt.o</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>tx_timer_initialize.o</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>tx_initialize_low_level.o</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>main.o</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>stm32l4xx_hal_i2c_ex.o</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>tx_timer_initialize.o</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="27">
                   <c:v>tx_byte_pool_create.o</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>tx_thread_schedule.o</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="28">
+                  <c:v>gpio.o</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>tx_thread_sleep.o</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>tx_timer_system_activate.o</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>tx_timer_interrupt.o</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>main.o</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>gpio.o</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>rx8900_callout.o</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>tx_initialize_low_level.o</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>tx_thread_time_slice.o</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>__scatter.o</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>tx_timer_system_activate.o</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>rx8900_callout.o</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>tx_thread_shell_entry.o</c:v>
                 </c:pt>
-                <c:pt idx="32">
-                  <c:v>tx_initialize_high_level.o</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>tx_thread_initialize.o</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>stm32l4xx_hal_pwr.o</c:v>
-                </c:pt>
                 <c:pt idx="35">
-                  <c:v>tx_timer_system_deactivate.o</c:v>
+                  <c:v>system_stm32l4xx.o</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>app_azure_rtos.o</c:v>
                 </c:pt>
                 <c:pt idx="37">
+                  <c:v>appirqcallout.o</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>rt_memclr_w.o</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>tx_initialize_kernel_enter.o</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="40">
+                  <c:v>sys_stackheap_outer.o</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>stm32l4xx_hal_pwr.o</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>tx_thread_timeout.o</c:v>
                 </c:pt>
-                <c:pt idx="39">
-                  <c:v>__scatter.o</c:v>
-                </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="43">
+                  <c:v>rt_memclr.o</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>tx_thread_stack_build.o</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>tx_timer_system_deactivate.o</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>tx_thread_initialize.o</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>stm32l4xx_hal.o</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>stm32l4xx_hal_msp.o</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>tx_initialize_high_level.o</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>app_threadx.o</c:v>
                 </c:pt>
-                <c:pt idx="41">
-                  <c:v>system_stm32l4xx.o</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>rt_memclr_w.o</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>sys_stackheap_outer.o</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>stm32l4xx_hal.o</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>rt_memclr.o</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>stm32l4xx_hal_msp.o</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>tx_thread_stack_build.o</c:v>
-                </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="51">
                   <c:v>tx_timer_expiration_process.o</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="52">
                   <c:v>tx_thread_system_return.o</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="53">
+                  <c:v>stm32l4xx_it.o</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>__scatter_zi.o</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>fz_wm.l</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>fpinit.o</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>__scatter_copy.o</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>tx_time_set.o</c:v>
+                </c:pt>
+                <c:pt idx="59">
                   <c:v>tx_time_get.o</c:v>
                 </c:pt>
-                <c:pt idx="51">
-                  <c:v>stm32l4xx_it.o</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>__scatter_zi.o</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>appirqcallout.o</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>fz_wm.l</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>fpinit.o</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>__scatter_copy.o</c:v>
-                </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="60">
                   <c:v>exit.o</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="61">
                   <c:v>aeabi_memset.o</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="62">
                   <c:v>tx_thread_interrupt_disable.o</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="63">
                   <c:v>sys_exit.o</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="64">
                   <c:v>__rtentry2.o</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="65">
                   <c:v>rtexit2.o</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="66">
                   <c:v>libspace.o</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="67">
                   <c:v>__main.o</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="68">
                   <c:v>libinit2.o</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="69">
                   <c:v>heapauxi.o</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="70">
                   <c:v>__rtentry4.o</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="71">
                   <c:v>tx_thread_interrupt_restore.o</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="72">
                   <c:v>rx8900_lcfg.o</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="73">
                   <c:v>use_no_semi.o</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="74">
                   <c:v>rtexit.o</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="75">
                   <c:v>libshutdown2.o</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="76">
                   <c:v>libshutdown.o</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="77">
                   <c:v>libinit.o</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="78">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -765,236 +795,245 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flash_percent!$B$3:$B$78</c:f>
+              <c:f>flash_percent!$B$3:$B$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="76"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
-                  <c:v>18.26149940490723</c:v>
+                  <c:v>15.34411430358887</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.60677337646484</c:v>
+                  <c:v>11.81969547271729</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.505424976348877</c:v>
+                  <c:v>7.177779197692871</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.799131870269775</c:v>
+                  <c:v>5.50153112411499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.590775489807129</c:v>
+                  <c:v>5.232901573181152</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.165553331375122</c:v>
+                  <c:v>4.598936080932617</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.131515026092529</c:v>
+                  <c:v>4.512974739074707</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.484789133071899</c:v>
+                  <c:v>4.126148223876953</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.152916669845581</c:v>
+                  <c:v>2.578842639923096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.042292356491089</c:v>
+                  <c:v>2.471390962600708</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.016763925552368</c:v>
+                  <c:v>2.294095516204834</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.008254289627075</c:v>
+                  <c:v>2.11680006980896</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.957196950912476</c:v>
+                  <c:v>2.041583776473999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.73594856262207</c:v>
+                  <c:v>1.891151309013367</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.633834004402161</c:v>
+                  <c:v>1.78369951248169</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.591286182403565</c:v>
+                  <c:v>1.708483338356018</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.557247996330261</c:v>
+                  <c:v>1.633267045021057</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.506190657615662</c:v>
+                  <c:v>1.482834577560425</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.463642954826355</c:v>
+                  <c:v>1.35389244556427</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.335999608039856</c:v>
+                  <c:v>1.332402110099793</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.301961421966553</c:v>
+                  <c:v>1.09600818157196</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.233885049819946</c:v>
+                  <c:v>1.042282223701477</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.072203516960144</c:v>
+                  <c:v>0.9885563850402832</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.9615793824195862</c:v>
+                  <c:v>0.8596142530441284</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.9020125269889832</c:v>
+                  <c:v>0.8166335225105286</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.7828787565231323</c:v>
+                  <c:v>0.8166335225105286</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.7488405704498291</c:v>
+                  <c:v>0.7843980193138123</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.7233119010925293</c:v>
+                  <c:v>0.7306721210479736</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.6977832913398743</c:v>
+                  <c:v>0.7199269533157349</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.6467259526252747</c:v>
+                  <c:v>0.6662010550498962</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.6382163763046265</c:v>
+                  <c:v>0.6232203245162964</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.57014000415802</c:v>
+                  <c:v>0.5050233602523804</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.57014000415802</c:v>
+                  <c:v>0.4835330247879028</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.5531208515167236</c:v>
+                  <c:v>0.4835330247879028</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.5190826654434204</c:v>
+                  <c:v>0.4727878272533417</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.476534903049469</c:v>
+                  <c:v>0.4620426595211029</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.4552610218524933</c:v>
+                  <c:v>0.4512974917888641</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.4424967169761658</c:v>
+                  <c:v>0.440552294254303</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.4084585011005402</c:v>
+                  <c:v>0.4190619587898254</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.3999489545822144</c:v>
+                  <c:v>0.4190619587898254</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.3999489545822144</c:v>
+                  <c:v>0.3975715935230255</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.3659107387065888</c:v>
+                  <c:v>0.3975715935230255</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.3318725228309631</c:v>
+                  <c:v>0.3868264257907867</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.3148534297943115</c:v>
+                  <c:v>0.3653360605239868</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.3063438832759857</c:v>
+                  <c:v>0.3438456952571869</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.2893247604370117</c:v>
+                  <c:v>0.3116101622581482</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.2808152139186859</c:v>
+                  <c:v>0.3116101622581482</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.2723056674003601</c:v>
+                  <c:v>0.3008649945259094</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.1957196891307831</c:v>
+                  <c:v>0.2686294615268707</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.1616814881563187</c:v>
+                  <c:v>0.2471390962600708</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.1446623802185059</c:v>
+                  <c:v>0.2363939136266708</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.1361528337001801</c:v>
+                  <c:v>0.2149035632610321</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.1191337257623673</c:v>
+                  <c:v>0.2041583806276321</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.1191337257623673</c:v>
+                  <c:v>0.1611776649951935</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.1106241792440414</c:v>
+                  <c:v>0.1504324972629547</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.1106241792440414</c:v>
+                  <c:v>0.1396873146295548</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.1106241792440414</c:v>
+                  <c:v>0.1396873146295548</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.07658597081899643</c:v>
+                  <c:v>0.1396873146295548</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.06807641685009003</c:v>
+                  <c:v>0.1396873146295548</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.05956686288118362</c:v>
+                  <c:v>0.1289421319961548</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.05105731263756752</c:v>
+                  <c:v>0.09670660644769669</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.05105731263756752</c:v>
+                  <c:v>0.08596142381429672</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.04254775866866112</c:v>
+                  <c:v>0.07521624863147736</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.03403820842504501</c:v>
+                  <c:v>0.06447106599807739</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.03403820842504501</c:v>
+                  <c:v>0.06447106599807739</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.02552865631878376</c:v>
+                  <c:v>0.05372589081525803</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.02552865631878376</c:v>
+                  <c:v>0.04298071190714836</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.02552865631878376</c:v>
+                  <c:v>0.04298071190714836</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.02552865631878376</c:v>
+                  <c:v>0.0322355329990387</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.01701910421252251</c:v>
+                  <c:v>0.0322355329990387</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.008509552106261253</c:v>
+                  <c:v>0.0322355329990387</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.008509552106261253</c:v>
+                  <c:v>0.0322355329990387</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.008509552106261253</c:v>
+                  <c:v>0.02149035595357418</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.008509552106261253</c:v>
+                  <c:v>0.01074517797678709</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.008509552106261253</c:v>
+                  <c:v>0.01074517797678709</c:v>
                 </c:pt>
                 <c:pt idx="75">
+                  <c:v>0.01074517797678709</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.01074517797678709</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.01074517797678709</c:v>
+                </c:pt>
+                <c:pt idx="78">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1099,8 +1138,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H78" totalsRowCount="1">
-  <autoFilter ref="A2:H77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H81" totalsRowCount="1">
+  <autoFilter ref="A2:H80"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="ram_percent" totalsRowFunction="sum"/>
@@ -1116,8 +1155,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H78" totalsRowCount="1">
-  <autoFilter ref="A2:H77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H81" totalsRowCount="1">
+  <autoFilter ref="A2:H80"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="flash_percent" totalsRowFunction="sum"/>
@@ -1417,7 +1456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1433,28 +1472,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1462,7 +1501,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>32.57688140869141</v>
+        <v>32.15407180786133</v>
       </c>
       <c r="C3" s="1">
         <v>1536</v>
@@ -1488,25 +1527,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>25.76882362365723</v>
+        <v>25.30877113342285</v>
       </c>
       <c r="C4" s="1">
-        <v>1215</v>
+        <v>1209</v>
       </c>
       <c r="D4" s="1">
-        <v>374</v>
+        <v>427</v>
       </c>
       <c r="E4" s="1">
-        <v>360</v>
+        <v>426</v>
       </c>
       <c r="F4" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1">
-        <v>1215</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1514,19 +1553,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>18.40933227539063</v>
+        <v>18.17040061950684</v>
       </c>
       <c r="C5" s="1">
         <v>868</v>
       </c>
       <c r="D5" s="1">
-        <v>306</v>
+        <v>160</v>
       </c>
       <c r="E5" s="1">
-        <v>286</v>
+        <v>160</v>
       </c>
       <c r="F5" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -1540,19 +1579,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>11.96182441711426</v>
+        <v>11.80657291412354</v>
       </c>
       <c r="C6" s="1">
         <v>564</v>
       </c>
       <c r="D6" s="1">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="E6" s="1">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F6" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -1566,16 +1605,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>3.647932052612305</v>
+        <v>3.600586175918579</v>
       </c>
       <c r="C7" s="1">
         <v>172</v>
       </c>
       <c r="D7" s="1">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1">
-        <v>126</v>
+        <v>54</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -1592,7 +1631,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>2.036055088043213</v>
+        <v>2.009629487991333</v>
       </c>
       <c r="C8" s="1">
         <v>96</v>
@@ -1618,7 +1657,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>2.036055088043213</v>
+        <v>2.009629487991333</v>
       </c>
       <c r="C9" s="1">
         <v>96</v>
@@ -1644,16 +1683,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>1.781548261642456</v>
+        <v>1.758425831794739</v>
       </c>
       <c r="C10" s="1">
         <v>84</v>
       </c>
       <c r="D10" s="1">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="E10" s="1">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1670,16 +1709,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>1.102863192558289</v>
+        <v>1.172283887863159</v>
       </c>
       <c r="C11" s="1">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D11" s="1">
-        <v>134</v>
+        <v>204</v>
       </c>
       <c r="E11" s="1">
-        <v>134</v>
+        <v>204</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1688,7 +1727,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1696,16 +1735,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>0.2545068860054016</v>
+        <v>1.088549256324768</v>
       </c>
       <c r="C12" s="1">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1">
-        <v>366</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1">
-        <v>366</v>
+        <v>46</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1714,7 +1753,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>12</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1722,16 +1761,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>0.1696712672710419</v>
+        <v>0.334938257932663</v>
       </c>
       <c r="C13" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1">
-        <v>1598</v>
+        <v>840</v>
       </c>
       <c r="E13" s="1">
-        <v>1598</v>
+        <v>840</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1740,7 +1779,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1748,25 +1787,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>0.08483563363552094</v>
+        <v>0.1674691289663315</v>
       </c>
       <c r="C14" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D14" s="1">
-        <v>736</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1">
-        <v>736</v>
+        <v>48</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H14" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1774,25 +1813,25 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>0.08483563363552094</v>
+        <v>0.1674691289663315</v>
       </c>
       <c r="C15" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1">
-        <v>86</v>
+        <v>1024</v>
       </c>
       <c r="E15" s="1">
-        <v>18</v>
+        <v>1024</v>
       </c>
       <c r="F15" s="1">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1800,56 +1839,108 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>0.08483563363552094</v>
+        <v>0.08373456448316574</v>
       </c>
       <c r="C16" s="1">
         <v>4</v>
       </c>
       <c r="D16" s="1">
-        <v>72</v>
+        <v>856</v>
       </c>
       <c r="E16" s="1">
-        <v>68</v>
+        <v>856</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
       </c>
       <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
         <v>4</v>
       </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8">
-      <c r="A78" t="s">
-        <v>77</v>
-      </c>
-      <c r="B78">
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.08373456448316574</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>86</v>
+      </c>
+      <c r="E17" s="1">
+        <v>18</v>
+      </c>
+      <c r="F17" s="1">
+        <v>64</v>
+      </c>
+      <c r="G17" s="1">
+        <v>4</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.08373456448316574</v>
+      </c>
+      <c r="C18" s="1">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1">
+        <v>82</v>
+      </c>
+      <c r="E18" s="1">
+        <v>82</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81">
         <f>SUBTOTAL(109,[ram_percent])</f>
         <v>0</v>
       </c>
-      <c r="C78">
+      <c r="C81">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="D78">
+      <c r="D81">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="E78">
+      <c r="E81">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F78">
+      <c r="F81">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G78">
+      <c r="G81">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H78">
+      <c r="H81">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>
@@ -1865,7 +1956,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1881,45 +1972,45 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
         <v>85</v>
       </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" t="s">
-        <v>82</v>
-      </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2">
-        <v>18.26149940490723</v>
+        <v>15.34411430358887</v>
       </c>
       <c r="C3" s="1">
-        <v>4292</v>
+        <v>2856</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>4292</v>
+        <v>2856</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -1933,19 +2024,19 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2">
-        <v>13.60677337646484</v>
+        <v>11.81969547271729</v>
       </c>
       <c r="C4" s="1">
-        <v>3198</v>
+        <v>2200</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>3198</v>
+        <v>2200</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1959,19 +2050,19 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2">
-        <v>7.505424976348877</v>
+        <v>7.177779197692871</v>
       </c>
       <c r="C5" s="1">
-        <v>1764</v>
+        <v>1336</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>1764</v>
+        <v>1336</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -1985,19 +2076,19 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2">
-        <v>6.799131870269775</v>
+        <v>5.50153112411499</v>
       </c>
       <c r="C6" s="1">
-        <v>1598</v>
+        <v>1024</v>
       </c>
       <c r="D6" s="1">
         <v>8</v>
       </c>
       <c r="E6" s="1">
-        <v>1598</v>
+        <v>1024</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -2011,19 +2102,19 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
-        <v>5.590775489807129</v>
+        <v>5.232901573181152</v>
       </c>
       <c r="C7" s="1">
-        <v>1314</v>
+        <v>974</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>1314</v>
+        <v>974</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -2037,19 +2128,19 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
-        <v>3.165553331375122</v>
+        <v>4.598936080932617</v>
       </c>
       <c r="C8" s="1">
-        <v>744</v>
+        <v>856</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E8" s="1">
-        <v>744</v>
+        <v>856</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -2058,24 +2149,24 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>3.131515026092529</v>
+        <v>4.512974739074707</v>
       </c>
       <c r="C9" s="1">
-        <v>736</v>
+        <v>840</v>
       </c>
       <c r="D9" s="1">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1">
-        <v>736</v>
+        <v>840</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -2084,24 +2175,24 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
-        <v>2.484789133071899</v>
+        <v>4.126148223876953</v>
       </c>
       <c r="C10" s="1">
-        <v>584</v>
+        <v>768</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>584</v>
+        <v>768</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -2115,19 +2206,19 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2">
-        <v>2.152916669845581</v>
+        <v>2.578842639923096</v>
       </c>
       <c r="C11" s="1">
-        <v>506</v>
+        <v>480</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="E11" s="1">
-        <v>506</v>
+        <v>480</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -2136,76 +2227,76 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2">
-        <v>2.042292356491089</v>
+        <v>2.471390962600708</v>
       </c>
       <c r="C12" s="1">
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="D12" s="1">
-        <v>96</v>
+        <v>1536</v>
       </c>
       <c r="E12" s="1">
-        <v>480</v>
+        <v>64</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>396</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>96</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B13" s="2">
-        <v>2.016763925552368</v>
+        <v>2.294095516204834</v>
       </c>
       <c r="C13" s="1">
-        <v>474</v>
+        <v>427</v>
       </c>
       <c r="D13" s="1">
-        <v>0</v>
+        <v>1209</v>
       </c>
       <c r="E13" s="1">
-        <v>474</v>
+        <v>426</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
-        <v>2.008254289627075</v>
+        <v>2.11680006980896</v>
       </c>
       <c r="C14" s="1">
-        <v>472</v>
+        <v>394</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>472</v>
+        <v>394</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -2219,28 +2310,28 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2">
-        <v>1.957196950912476</v>
+        <v>2.041583776473999</v>
       </c>
       <c r="C15" s="1">
-        <v>460</v>
+        <v>380</v>
       </c>
       <c r="D15" s="1">
-        <v>1536</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>64</v>
+        <v>380</v>
       </c>
       <c r="F15" s="1">
-        <v>396</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>1536</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2248,16 +2339,16 @@
         <v>24</v>
       </c>
       <c r="B16" s="2">
-        <v>1.73594856262207</v>
+        <v>1.891151309013367</v>
       </c>
       <c r="C16" s="1">
-        <v>408</v>
+        <v>352</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>408</v>
+        <v>352</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -2274,16 +2365,16 @@
         <v>25</v>
       </c>
       <c r="B17" s="2">
-        <v>1.633834004402161</v>
+        <v>1.78369951248169</v>
       </c>
       <c r="C17" s="1">
-        <v>384</v>
+        <v>332</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>384</v>
+        <v>332</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -2297,45 +2388,45 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2">
-        <v>1.591286182403565</v>
+        <v>1.708483338356018</v>
       </c>
       <c r="C18" s="1">
-        <v>374</v>
+        <v>318</v>
       </c>
       <c r="D18" s="1">
-        <v>1215</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>360</v>
+        <v>318</v>
       </c>
       <c r="F18" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>1215</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19" s="2">
-        <v>1.557247996330261</v>
+        <v>1.633267045021057</v>
       </c>
       <c r="C19" s="1">
-        <v>366</v>
+        <v>304</v>
       </c>
       <c r="D19" s="1">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="E19" s="1">
-        <v>366</v>
+        <v>304</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -2344,24 +2435,24 @@
         <v>0</v>
       </c>
       <c r="H19" s="1">
-        <v>12</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2">
-        <v>1.506190657615662</v>
+        <v>1.482834577560425</v>
       </c>
       <c r="C20" s="1">
-        <v>354</v>
+        <v>276</v>
       </c>
       <c r="D20" s="1">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>354</v>
+        <v>276</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -2370,24 +2461,24 @@
         <v>0</v>
       </c>
       <c r="H20" s="1">
-        <v>84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2">
-        <v>1.463642954826355</v>
+        <v>1.35389244556427</v>
       </c>
       <c r="C21" s="1">
-        <v>344</v>
+        <v>252</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>344</v>
+        <v>252</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -2401,19 +2492,19 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2">
-        <v>1.335999608039856</v>
+        <v>1.332402110099793</v>
       </c>
       <c r="C22" s="1">
-        <v>314</v>
+        <v>248</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>314</v>
+        <v>248</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -2427,45 +2518,45 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B23" s="2">
-        <v>1.301961421966553</v>
+        <v>1.09600818157196</v>
       </c>
       <c r="C23" s="1">
-        <v>306</v>
+        <v>204</v>
       </c>
       <c r="D23" s="1">
-        <v>868</v>
+        <v>56</v>
       </c>
       <c r="E23" s="1">
-        <v>286</v>
+        <v>204</v>
       </c>
       <c r="F23" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>868</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B24" s="2">
-        <v>1.233885049819946</v>
+        <v>1.042282223701477</v>
       </c>
       <c r="C24" s="1">
-        <v>290</v>
+        <v>194</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>290</v>
+        <v>194</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -2479,19 +2570,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2">
-        <v>1.072203516960144</v>
+        <v>0.9885563850402832</v>
       </c>
       <c r="C25" s="1">
-        <v>252</v>
+        <v>184</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>252</v>
+        <v>184</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -2505,19 +2596,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B26" s="2">
-        <v>0.9615793824195862</v>
+        <v>0.8596142530441284</v>
       </c>
       <c r="C26" s="1">
-        <v>226</v>
+        <v>160</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>868</v>
       </c>
       <c r="E26" s="1">
-        <v>226</v>
+        <v>160</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -2526,24 +2617,24 @@
         <v>0</v>
       </c>
       <c r="H26" s="1">
-        <v>0</v>
+        <v>868</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2">
-        <v>0.9020125269889832</v>
+        <v>0.8166335225105286</v>
       </c>
       <c r="C27" s="1">
-        <v>212</v>
+        <v>152</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>212</v>
+        <v>152</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -2557,19 +2648,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28" s="2">
-        <v>0.7828787565231323</v>
+        <v>0.8166335225105286</v>
       </c>
       <c r="C28" s="1">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -2583,19 +2674,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" s="2">
-        <v>0.7488405704498291</v>
+        <v>0.7843980193138123</v>
       </c>
       <c r="C29" s="1">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -2609,19 +2700,19 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B30" s="2">
-        <v>0.7233119010925293</v>
+        <v>0.7306721210479736</v>
       </c>
       <c r="C30" s="1">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -2635,19 +2726,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31" s="2">
-        <v>0.6977832913398743</v>
+        <v>0.7199269533157349</v>
       </c>
       <c r="C31" s="1">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -2661,19 +2752,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32" s="2">
-        <v>0.6467259526252747</v>
+        <v>0.6662010550498962</v>
       </c>
       <c r="C32" s="1">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -2687,19 +2778,19 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B33" s="2">
-        <v>0.6382163763046265</v>
+        <v>0.6232203245162964</v>
       </c>
       <c r="C33" s="1">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
@@ -2713,19 +2804,19 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2">
-        <v>0.57014000415802</v>
+        <v>0.5050233602523804</v>
       </c>
       <c r="C34" s="1">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
       </c>
       <c r="E34" s="1">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="F34" s="1">
         <v>0</v>
@@ -2739,19 +2830,19 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2">
-        <v>0.57014000415802</v>
+        <v>0.4835330247879028</v>
       </c>
       <c r="C35" s="1">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="D35" s="1">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
@@ -2760,50 +2851,50 @@
         <v>0</v>
       </c>
       <c r="H35" s="1">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B36" s="2">
-        <v>0.5531208515167236</v>
+        <v>0.4835330247879028</v>
       </c>
       <c r="C36" s="1">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="D36" s="1">
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
       </c>
       <c r="G36" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H36" s="1">
-        <v>168</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B37" s="2">
-        <v>0.5190826654434204</v>
+        <v>0.4727878272533417</v>
       </c>
       <c r="C37" s="1">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -2817,25 +2908,25 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B38" s="2">
-        <v>0.476534903049469</v>
+        <v>0.4620426595211029</v>
       </c>
       <c r="C38" s="1">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="D38" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E38" s="1">
-        <v>112</v>
+        <v>18</v>
       </c>
       <c r="F38" s="1">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="G38" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H38" s="1">
         <v>0</v>
@@ -2846,19 +2937,19 @@
         <v>4</v>
       </c>
       <c r="B39" s="2">
-        <v>0.4552610218524933</v>
+        <v>0.4512974917888641</v>
       </c>
       <c r="C39" s="1">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="D39" s="1">
         <v>564</v>
       </c>
       <c r="E39" s="1">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F39" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G39" s="1">
         <v>0</v>
@@ -2869,19 +2960,19 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B40" s="2">
-        <v>0.4424967169761658</v>
+        <v>0.440552294254303</v>
       </c>
       <c r="C40" s="1">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D40" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E40" s="1">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
@@ -2890,24 +2981,24 @@
         <v>0</v>
       </c>
       <c r="H40" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B41" s="2">
-        <v>0.4084585011005402</v>
+        <v>0.4190619587898254</v>
       </c>
       <c r="C41" s="1">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
@@ -2921,19 +3012,19 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B42" s="2">
-        <v>0.3999489545822144</v>
+        <v>0.4190619587898254</v>
       </c>
       <c r="C42" s="1">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F42" s="1">
         <v>0</v>
@@ -2947,19 +3038,19 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B43" s="2">
-        <v>0.3999489545822144</v>
+        <v>0.3975715935230255</v>
       </c>
       <c r="C43" s="1">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
       </c>
       <c r="E43" s="1">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="F43" s="1">
         <v>0</v>
@@ -2973,25 +3064,25 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B44" s="2">
-        <v>0.3659107387065888</v>
+        <v>0.3975715935230255</v>
       </c>
       <c r="C44" s="1">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D44" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E44" s="1">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="F44" s="1">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="G44" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H44" s="1">
         <v>0</v>
@@ -2999,19 +3090,19 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B45" s="2">
-        <v>0.3318725228309631</v>
+        <v>0.3868264257907867</v>
       </c>
       <c r="C45" s="1">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D45" s="1">
         <v>0</v>
       </c>
       <c r="E45" s="1">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F45" s="1">
         <v>0</v>
@@ -3025,19 +3116,19 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B46" s="2">
-        <v>0.3148534297943115</v>
+        <v>0.3653360605239868</v>
       </c>
       <c r="C46" s="1">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
       </c>
       <c r="E46" s="1">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F46" s="1">
         <v>0</v>
@@ -3051,25 +3142,25 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="B47" s="2">
-        <v>0.3063438832759857</v>
+        <v>0.3438456952571869</v>
       </c>
       <c r="C47" s="1">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D47" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E47" s="1">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F47" s="1">
         <v>0</v>
       </c>
       <c r="G47" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H47" s="1">
         <v>0</v>
@@ -3077,19 +3168,19 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B48" s="2">
-        <v>0.2893247604370117</v>
+        <v>0.3116101622581482</v>
       </c>
       <c r="C48" s="1">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
       </c>
       <c r="E48" s="1">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F48" s="1">
         <v>0</v>
@@ -3103,51 +3194,51 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="B49" s="2">
-        <v>0.2808152139186859</v>
+        <v>0.3116101622581482</v>
       </c>
       <c r="C49" s="1">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D49" s="1">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="E49" s="1">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="F49" s="1">
         <v>0</v>
       </c>
       <c r="G49" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H49" s="1">
-        <v>0</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="B50" s="2">
-        <v>0.2723056674003601</v>
+        <v>0.3008649945259094</v>
       </c>
       <c r="C50" s="1">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D50" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E50" s="1">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F50" s="1">
         <v>0</v>
       </c>
       <c r="G50" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H50" s="1">
         <v>0</v>
@@ -3155,19 +3246,19 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="2">
+        <v>0.2686294615268707</v>
+      </c>
+      <c r="C51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="2">
-        <v>0.1957196891307831</v>
-      </c>
-      <c r="C51" s="1">
-        <v>46</v>
-      </c>
       <c r="D51" s="1">
         <v>0</v>
       </c>
       <c r="E51" s="1">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
@@ -3181,19 +3272,19 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="B52" s="2">
-        <v>0.1616814881563187</v>
+        <v>0.2471390962600708</v>
       </c>
       <c r="C52" s="1">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D52" s="1">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E52" s="1">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F52" s="1">
         <v>0</v>
@@ -3202,7 +3293,7 @@
         <v>0</v>
       </c>
       <c r="H52" s="1">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3210,16 +3301,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>0.1446623802185059</v>
+        <v>0.2363939136266708</v>
       </c>
       <c r="C53" s="1">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
       </c>
       <c r="E53" s="1">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F53" s="1">
         <v>0</v>
@@ -3236,16 +3327,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>0.1361528337001801</v>
+        <v>0.2149035632610321</v>
       </c>
       <c r="C54" s="1">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D54" s="1">
         <v>0</v>
       </c>
       <c r="E54" s="1">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F54" s="1">
         <v>0</v>
@@ -3262,16 +3353,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="2">
-        <v>0.1191337257623673</v>
+        <v>0.2041583806276321</v>
       </c>
       <c r="C55" s="1">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
       </c>
       <c r="E55" s="1">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F55" s="1">
         <v>0</v>
@@ -3288,16 +3379,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="2">
-        <v>0.1191337257623673</v>
+        <v>0.1611776649951935</v>
       </c>
       <c r="C56" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
       </c>
       <c r="E56" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
@@ -3314,16 +3405,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="2">
-        <v>0.1106241792440414</v>
+        <v>0.1504324972629547</v>
       </c>
       <c r="C57" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
       </c>
       <c r="E57" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
@@ -3340,7 +3431,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>0.1106241792440414</v>
+        <v>0.1396873146295548</v>
       </c>
       <c r="C58" s="1">
         <v>26</v>
@@ -3366,7 +3457,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="2">
-        <v>0.1106241792440414</v>
+        <v>0.1396873146295548</v>
       </c>
       <c r="C59" s="1">
         <v>26</v>
@@ -3392,16 +3483,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>0.07658597081899643</v>
+        <v>0.1396873146295548</v>
       </c>
       <c r="C60" s="1">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D60" s="1">
         <v>0</v>
       </c>
       <c r="E60" s="1">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F60" s="1">
         <v>0</v>
@@ -3418,16 +3509,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="2">
-        <v>0.06807641685009003</v>
+        <v>0.1396873146295548</v>
       </c>
       <c r="C61" s="1">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D61" s="1">
         <v>0</v>
       </c>
       <c r="E61" s="1">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F61" s="1">
         <v>0</v>
@@ -3444,16 +3535,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="2">
-        <v>0.05956686288118362</v>
+        <v>0.1289421319961548</v>
       </c>
       <c r="C62" s="1">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D62" s="1">
         <v>0</v>
       </c>
       <c r="E62" s="1">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F62" s="1">
         <v>0</v>
@@ -3470,16 +3561,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="2">
-        <v>0.05105731263756752</v>
+        <v>0.09670660644769669</v>
       </c>
       <c r="C63" s="1">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D63" s="1">
         <v>0</v>
       </c>
       <c r="E63" s="1">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F63" s="1">
         <v>0</v>
@@ -3496,16 +3587,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="2">
-        <v>0.05105731263756752</v>
+        <v>0.08596142381429672</v>
       </c>
       <c r="C64" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D64" s="1">
         <v>0</v>
       </c>
       <c r="E64" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F64" s="1">
         <v>0</v>
@@ -3522,16 +3613,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="2">
-        <v>0.04254775866866112</v>
+        <v>0.07521624863147736</v>
       </c>
       <c r="C65" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D65" s="1">
         <v>0</v>
       </c>
       <c r="E65" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F65" s="1">
         <v>0</v>
@@ -3545,19 +3636,19 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B66" s="2">
-        <v>0.03403820842504501</v>
+        <v>0.06447106599807739</v>
       </c>
       <c r="C66" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D66" s="1">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="E66" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F66" s="1">
         <v>0</v>
@@ -3566,24 +3657,24 @@
         <v>0</v>
       </c>
       <c r="H66" s="1">
-        <v>96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B67" s="2">
-        <v>0.03403820842504501</v>
+        <v>0.06447106599807739</v>
       </c>
       <c r="C67" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D67" s="1">
         <v>0</v>
       </c>
       <c r="E67" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F67" s="1">
         <v>0</v>
@@ -3597,19 +3688,19 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B68" s="2">
-        <v>0.02552865631878376</v>
+        <v>0.05372589081525803</v>
       </c>
       <c r="C68" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D68" s="1">
         <v>0</v>
       </c>
       <c r="E68" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F68" s="1">
         <v>0</v>
@@ -3623,19 +3714,19 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="B69" s="2">
-        <v>0.02552865631878376</v>
+        <v>0.04298071190714836</v>
       </c>
       <c r="C69" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D69" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="E69" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F69" s="1">
         <v>0</v>
@@ -3644,7 +3735,7 @@
         <v>0</v>
       </c>
       <c r="H69" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3652,16 +3743,16 @@
         <v>68</v>
       </c>
       <c r="B70" s="2">
-        <v>0.02552865631878376</v>
+        <v>0.04298071190714836</v>
       </c>
       <c r="C70" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D70" s="1">
         <v>0</v>
       </c>
       <c r="E70" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F70" s="1">
         <v>0</v>
@@ -3678,7 +3769,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="2">
-        <v>0.02552865631878376</v>
+        <v>0.0322355329990387</v>
       </c>
       <c r="C71" s="1">
         <v>6</v>
@@ -3704,19 +3795,19 @@
         <v>70</v>
       </c>
       <c r="B72" s="2">
-        <v>0.01701910421252251</v>
+        <v>0.0322355329990387</v>
       </c>
       <c r="C72" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D72" s="1">
         <v>0</v>
       </c>
       <c r="E72" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F72" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G72" s="1">
         <v>0</v>
@@ -3730,16 +3821,16 @@
         <v>71</v>
       </c>
       <c r="B73" s="2">
-        <v>0.008509552106261253</v>
+        <v>0.0322355329990387</v>
       </c>
       <c r="C73" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
       </c>
       <c r="E73" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F73" s="1">
         <v>0</v>
@@ -3756,16 +3847,16 @@
         <v>72</v>
       </c>
       <c r="B74" s="2">
-        <v>0.008509552106261253</v>
+        <v>0.0322355329990387</v>
       </c>
       <c r="C74" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D74" s="1">
         <v>0</v>
       </c>
       <c r="E74" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F74" s="1">
         <v>0</v>
@@ -3782,19 +3873,19 @@
         <v>73</v>
       </c>
       <c r="B75" s="2">
-        <v>0.008509552106261253</v>
+        <v>0.02149035595357418</v>
       </c>
       <c r="C75" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D75" s="1">
         <v>0</v>
       </c>
       <c r="E75" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F75" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G75" s="1">
         <v>0</v>
@@ -3808,7 +3899,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="2">
-        <v>0.008509552106261253</v>
+        <v>0.01074517797678709</v>
       </c>
       <c r="C76" s="1">
         <v>2</v>
@@ -3834,7 +3925,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="2">
-        <v>0.008509552106261253</v>
+        <v>0.01074517797678709</v>
       </c>
       <c r="C77" s="1">
         <v>2</v>
@@ -3856,34 +3947,112 @@
       </c>
     </row>
     <row r="78" spans="1:8">
-      <c r="A78" t="s">
+      <c r="A78" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0.01074517797678709</v>
+      </c>
+      <c r="C78" s="1">
+        <v>2</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1">
+        <v>2</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1">
+        <v>0</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B78">
+      <c r="B79" s="2">
+        <v>0.01074517797678709</v>
+      </c>
+      <c r="C79" s="1">
+        <v>2</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0</v>
+      </c>
+      <c r="E79" s="1">
+        <v>2</v>
+      </c>
+      <c r="F79" s="1">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0</v>
+      </c>
+      <c r="H79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B80" s="2">
+        <v>0.01074517797678709</v>
+      </c>
+      <c r="C80" s="1">
+        <v>2</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0</v>
+      </c>
+      <c r="E80" s="1">
+        <v>2</v>
+      </c>
+      <c r="F80" s="1">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1">
+        <v>0</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81">
         <f>SUBTOTAL(109,[flash_percent])</f>
         <v>0</v>
       </c>
-      <c r="C78">
+      <c r="C81">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="D78">
+      <c r="D81">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="E78">
+      <c r="E81">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F78">
+      <c r="F81">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G78">
+      <c r="G81">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H78">
+      <c r="H81">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
add AppModeCtrl appobj htu21d
</commit_message>
<xml_diff>
--- a/Software/MDK-ARM/Software_analysis.xlsx
+++ b/Software/MDK-ARM/Software_analysis.xlsx
@@ -15,17 +15,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="98">
   <si>
     <t>Software</t>
   </si>
   <si>
+    <t>appmain.o</t>
+  </si>
+  <si>
     <t>startup_stm32l432xx.o</t>
   </si>
   <si>
-    <t>appmain.o</t>
-  </si>
-  <si>
     <t>tx_timer_initialize.o</t>
   </si>
   <si>
@@ -50,24 +50,27 @@
     <t>tx_initialize_high_level.o</t>
   </si>
   <si>
+    <t>appobj.o</t>
+  </si>
+  <si>
     <t>applowpowermgr.o</t>
   </si>
   <si>
+    <t>rx8900.o</t>
+  </si>
+  <si>
+    <t>appirqcallout.o</t>
+  </si>
+  <si>
+    <t>tx_low_power.o</t>
+  </si>
+  <si>
+    <t>system_stm32l4xx.o</t>
+  </si>
+  <si>
     <t>stm32l4xx_hal.o</t>
   </si>
   <si>
-    <t>rx8900.o</t>
-  </si>
-  <si>
-    <t>tx_low_power.o</t>
-  </si>
-  <si>
-    <t>system_stm32l4xx.o</t>
-  </si>
-  <si>
-    <t>appirqcallout.o</t>
-  </si>
-  <si>
     <t>stm32l4xx_hal_rcc.o</t>
   </si>
   <si>
@@ -83,106 +86,136 @@
     <t>stm32l4xx_hal_gpio.o</t>
   </si>
   <si>
+    <t>tx_event_flags_set.o</t>
+  </si>
+  <si>
+    <t>tx_thread_system_suspend.o</t>
+  </si>
+  <si>
     <t>txe_thread_create.o</t>
   </si>
   <si>
-    <t>tx_thread_system_suspend.o</t>
+    <t>tx_thread_create.o</t>
+  </si>
+  <si>
+    <t>tx_timer_thread_entry.o</t>
+  </si>
+  <si>
+    <t>tx_thread_system_resume.o</t>
+  </si>
+  <si>
+    <t>stm32l4xx_hal_cortex.o</t>
+  </si>
+  <si>
+    <t>tx_event_flags_get.o</t>
+  </si>
+  <si>
+    <t>stm32l4xx_hal_pwr_ex.o</t>
   </si>
   <si>
     <t>txe_byte_pool_create.o</t>
   </si>
   <si>
-    <t>tx_timer_thread_entry.o</t>
-  </si>
-  <si>
-    <t>tx_thread_create.o</t>
-  </si>
-  <si>
-    <t>stm32l4xx_hal_pwr_ex.o</t>
+    <t>stm32l4xx_hal_i2c_ex.o</t>
+  </si>
+  <si>
+    <t>txe_event_flags_create.o</t>
+  </si>
+  <si>
+    <t>tx_byte_pool_create.o</t>
+  </si>
+  <si>
+    <t>tx_event_flags_cleanup.o</t>
   </si>
   <si>
     <t>tx_thread_schedule.o</t>
   </si>
   <si>
-    <t>tx_thread_system_resume.o</t>
-  </si>
-  <si>
-    <t>stm32l4xx_hal_cortex.o</t>
+    <t>tx_thread_sleep.o</t>
+  </si>
+  <si>
+    <t>tx_timer_system_activate.o</t>
+  </si>
+  <si>
+    <t>txe_event_flags_get.o</t>
   </si>
   <si>
     <t>tx_timer_interrupt.o</t>
   </si>
   <si>
+    <t>main.o</t>
+  </si>
+  <si>
+    <t>gpio.o</t>
+  </si>
+  <si>
+    <t>rx8900_callout.o</t>
+  </si>
+  <si>
     <t>tx_initialize_low_level.o</t>
   </si>
   <si>
-    <t>main.o</t>
-  </si>
-  <si>
-    <t>stm32l4xx_hal_i2c_ex.o</t>
-  </si>
-  <si>
-    <t>tx_byte_pool_create.o</t>
-  </si>
-  <si>
-    <t>gpio.o</t>
-  </si>
-  <si>
-    <t>tx_thread_sleep.o</t>
-  </si>
-  <si>
     <t>tx_thread_time_slice.o</t>
   </si>
   <si>
+    <t>tx_event_flags_create.o</t>
+  </si>
+  <si>
+    <t>tx_thread_shell_entry.o</t>
+  </si>
+  <si>
+    <t>stm32l4xx_hal_pwr.o</t>
+  </si>
+  <si>
+    <t>tx_timer_system_deactivate.o</t>
+  </si>
+  <si>
+    <t>tx_initialize_kernel_enter.o</t>
+  </si>
+  <si>
+    <t>txe_event_flags_set.o</t>
+  </si>
+  <si>
+    <t>tx_thread_timeout.o</t>
+  </si>
+  <si>
     <t>__scatter.o</t>
   </si>
   <si>
-    <t>tx_timer_system_activate.o</t>
-  </si>
-  <si>
-    <t>rx8900_callout.o</t>
-  </si>
-  <si>
-    <t>tx_thread_shell_entry.o</t>
-  </si>
-  <si>
     <t>rt_memclr_w.o</t>
   </si>
   <si>
-    <t>tx_initialize_kernel_enter.o</t>
+    <t>app_threadx.o</t>
   </si>
   <si>
     <t>sys_stackheap_outer.o</t>
   </si>
   <si>
-    <t>stm32l4xx_hal_pwr.o</t>
-  </si>
-  <si>
-    <t>tx_thread_timeout.o</t>
-  </si>
-  <si>
     <t>rt_memclr.o</t>
   </si>
   <si>
+    <t>stm32l4xx_hal_msp.o</t>
+  </si>
+  <si>
     <t>tx_thread_stack_build.o</t>
   </si>
   <si>
-    <t>tx_timer_system_deactivate.o</t>
-  </si>
-  <si>
-    <t>stm32l4xx_hal_msp.o</t>
-  </si>
-  <si>
-    <t>app_threadx.o</t>
+    <t>stm32l4xx_it.o</t>
   </si>
   <si>
     <t>tx_timer_expiration_process.o</t>
   </si>
   <si>
+    <t>appmodectrl.o</t>
+  </si>
+  <si>
     <t>tx_thread_system_return.o</t>
   </si>
   <si>
-    <t>stm32l4xx_it.o</t>
+    <t>tx_time_set.o</t>
+  </si>
+  <si>
+    <t>tx_time_get.o</t>
   </si>
   <si>
     <t>__scatter_zi.o</t>
@@ -195,12 +228,6 @@
   </si>
   <si>
     <t>__scatter_copy.o</t>
-  </si>
-  <si>
-    <t>tx_time_set.o</t>
-  </si>
-  <si>
-    <t>tx_time_get.o</t>
   </si>
   <si>
     <t>exit.o</t>
@@ -371,14 +398,14 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ram_percent!$A$3:$A$81</c:f>
+              <c:f>ram_percent!$A$3:$A$90</c:f>
               <c:strCache>
-                <c:ptCount val="79"/>
+                <c:ptCount val="88"/>
                 <c:pt idx="0">
+                  <c:v>appmain.o</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>startup_stm32l432xx.o</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>appmain.o</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>tx_timer_initialize.o</c:v>
@@ -405,24 +432,27 @@
                   <c:v>tx_initialize_high_level.o</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>appobj.o</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>applowpowermgr.o</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>stm32l4xx_hal.o</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>rx8900.o</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>appirqcallout.o</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>tx_low_power.o</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>system_stm32l4xx.o</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>appirqcallout.o</c:v>
-                </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="16">
+                  <c:v>stm32l4xx_hal.o</c:v>
+                </c:pt>
+                <c:pt idx="87">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -430,59 +460,62 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ram_percent!$B$3:$B$81</c:f>
+              <c:f>ram_percent!$B$3:$B$90</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="79"/>
+                <c:ptCount val="88"/>
                 <c:pt idx="0">
-                  <c:v>32.14734268188477</c:v>
+                  <c:v>40.11637496948242</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.30347442626953</c:v>
+                  <c:v>25.53615951538086</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.16659736633301</c:v>
+                  <c:v>14.43059062957764</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.80410194396973</c:v>
+                  <c:v>9.376558303833008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.599832534790039</c:v>
+                  <c:v>2.859517812728882</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.009208917617798</c:v>
+                  <c:v>1.596009969711304</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.009208917617798</c:v>
+                  <c:v>1.596009969711304</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.758057713508606</c:v>
+                  <c:v>1.396508693695068</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.172038555145264</c:v>
+                  <c:v>0.9310058355331421</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.088321447372437</c:v>
+                  <c:v>0.864505410194397</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.3557974100112915</c:v>
+                  <c:v>0.5985037684440613</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1674340665340424</c:v>
+                  <c:v>0.2327514588832855</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1674340665340424</c:v>
+                  <c:v>0.133000835776329</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.08371703326702118</c:v>
+                  <c:v>0.133000835776329</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.08371703326702118</c:v>
+                  <c:v>0.06650041788816452</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.08371703326702118</c:v>
-                </c:pt>
-                <c:pt idx="78">
+                  <c:v>0.06650041788816452</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.06650041788816452</c:v>
+                </c:pt>
+                <c:pt idx="87">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -550,9 +583,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>flash_percent!$A$3:$A$81</c:f>
+              <c:f>flash_percent!$A$3:$A$90</c:f>
               <c:strCache>
-                <c:ptCount val="79"/>
+                <c:ptCount val="88"/>
                 <c:pt idx="0">
                   <c:v>stm32l4xx_hal_rcc.o</c:v>
                 </c:pt>
@@ -563,231 +596,258 @@
                   <c:v>stm32l4xx_hal_lptim.o</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>stm32l4xx_hal_rcc_ex.o</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>rx8900.o</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>stm32l4xx_hal_rcc_ex.o</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>applowpowermgr.o</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>stm32l4xx_hal_gpio.o</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tx_event_flags_set.o</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>tx_thread_system_suspend.o</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>tx_low_power.o</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>stm32l4xx_hal_gpio.o</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
+                  <c:v>txe_thread_create.o</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>appmain.o</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>tx_thread_create.o</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>c_w.l</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>startup_stm32l432xx.o</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>appmain.o</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>txe_thread_create.o</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>tx_thread_system_suspend.o</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>txe_byte_pool_create.o</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>tx_timer_thread_entry.o</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>tx_thread_create.o</c:v>
+                  <c:v>tx_thread_system_resume.o</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>stm32l4xx_hal_cortex.o</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>startup_stm32l432xx.o</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>tx_event_flags_get.o</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>stm32l4xx_hal_pwr_ex.o</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>i2c.o</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>stm32l4xx_hal_pwr_ex.o</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>tx_thread_schedule.o</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>tx_thread_system_resume.o</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>lptim.o</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>stm32l4xx_hal_cortex.o</c:v>
+                  <c:v>txe_byte_pool_create.o</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>tx_timer_interrupt.o</c:v>
+                  <c:v>stm32l4xx_hal_i2c_ex.o</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>tx_timer_initialize.o</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>tx_initialize_low_level.o</c:v>
+                  <c:v>txe_event_flags_create.o</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>main.o</c:v>
+                  <c:v>tx_byte_pool_create.o</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>stm32l4xx_hal_i2c_ex.o</c:v>
+                  <c:v>tx_event_flags_cleanup.o</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>tx_byte_pool_create.o</c:v>
+                  <c:v>tx_thread_schedule.o</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>gpio.o</c:v>
+                  <c:v>lptim.o</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>tx_thread_sleep.o</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>tx_timer_system_activate.o</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>txe_event_flags_get.o</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>tx_timer_interrupt.o</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>main.o</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>gpio.o</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>rx8900_callout.o</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>tx_initialize_low_level.o</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>tx_thread_time_slice.o</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="38">
+                  <c:v>tx_event_flags_create.o</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>tx_thread_shell_entry.o</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>tx_initialize_high_level.o</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>tx_thread_initialize.o</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>appirqcallout.o</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>stm32l4xx_hal_pwr.o</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>tx_timer_system_deactivate.o</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>app_azure_rtos.o</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>tx_initialize_kernel_enter.o</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>txe_event_flags_set.o</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>tx_thread_timeout.o</c:v>
+                </c:pt>
+                <c:pt idx="49">
                   <c:v>__scatter.o</c:v>
                 </c:pt>
-                <c:pt idx="32">
-                  <c:v>tx_timer_system_activate.o</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>rx8900_callout.o</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>tx_thread_shell_entry.o</c:v>
-                </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="50">
+                  <c:v>stm32l4xx_hal.o</c:v>
+                </c:pt>
+                <c:pt idx="51">
                   <c:v>system_stm32l4xx.o</c:v>
                 </c:pt>
-                <c:pt idx="36">
-                  <c:v>appirqcallout.o</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>app_azure_rtos.o</c:v>
-                </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="52">
                   <c:v>rt_memclr_w.o</c:v>
                 </c:pt>
-                <c:pt idx="39">
-                  <c:v>tx_initialize_kernel_enter.o</c:v>
-                </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="53">
+                  <c:v>app_threadx.o</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>sys_stackheap_outer.o</c:v>
                 </c:pt>
-                <c:pt idx="41">
-                  <c:v>stm32l4xx_hal_pwr.o</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>stm32l4xx_hal.o</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>tx_thread_timeout.o</c:v>
-                </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="55">
                   <c:v>rt_memclr.o</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="56">
+                  <c:v>stm32l4xx_hal_msp.o</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>appobj.o</c:v>
+                </c:pt>
+                <c:pt idx="58">
                   <c:v>tx_thread_stack_build.o</c:v>
                 </c:pt>
-                <c:pt idx="46">
-                  <c:v>tx_timer_system_deactivate.o</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>tx_thread_initialize.o</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>stm32l4xx_hal_msp.o</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>tx_initialize_high_level.o</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>app_threadx.o</c:v>
-                </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="59">
+                  <c:v>stm32l4xx_it.o</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>tx_timer_expiration_process.o</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="61">
+                  <c:v>appmodectrl.o</c:v>
+                </c:pt>
+                <c:pt idx="62">
                   <c:v>tx_thread_system_return.o</c:v>
                 </c:pt>
-                <c:pt idx="53">
-                  <c:v>stm32l4xx_it.o</c:v>
-                </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="63">
+                  <c:v>tx_time_set.o</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>tx_time_get.o</c:v>
+                </c:pt>
+                <c:pt idx="65">
                   <c:v>__scatter_zi.o</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="66">
                   <c:v>fz_wm.l</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="67">
                   <c:v>fpinit.o</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="68">
                   <c:v>__scatter_copy.o</c:v>
                 </c:pt>
-                <c:pt idx="58">
-                  <c:v>tx_time_set.o</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>tx_time_get.o</c:v>
-                </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="69">
                   <c:v>exit.o</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="70">
                   <c:v>aeabi_memset.o</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="71">
                   <c:v>tx_thread_interrupt_disable.o</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="72">
                   <c:v>sys_exit.o</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="73">
                   <c:v>__rtentry2.o</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="74">
                   <c:v>rtexit2.o</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="75">
                   <c:v>libspace.o</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="76">
                   <c:v>__main.o</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="77">
                   <c:v>libinit2.o</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="78">
                   <c:v>heapauxi.o</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="79">
                   <c:v>__rtentry4.o</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="80">
                   <c:v>tx_thread_interrupt_restore.o</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="81">
                   <c:v>rx8900_lcfg.o</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="82">
                   <c:v>use_no_semi.o</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="83">
                   <c:v>rtexit.o</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="84">
                   <c:v>libshutdown2.o</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="85">
                   <c:v>libshutdown.o</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="86">
                   <c:v>libinit.o</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="87">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -795,245 +855,272 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flash_percent!$B$3:$B$81</c:f>
+              <c:f>flash_percent!$B$3:$B$90</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="79"/>
+                <c:ptCount val="88"/>
                 <c:pt idx="0">
-                  <c:v>15.27191066741943</c:v>
+                  <c:v>13.3843994140625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.76407718658447</c:v>
+                  <c:v>10.93595027923584</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.144002914428711</c:v>
+                  <c:v>7.017064094543457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.475643157958984</c:v>
+                  <c:v>6.032212734222412</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.208277702331543</c:v>
+                  <c:v>5.464555740356445</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.775145530700684</c:v>
+                  <c:v>4.544677257537842</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.577295303344727</c:v>
+                  <c:v>4.363437175750732</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.106732368469238</c:v>
+                  <c:v>3.036624193191528</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.566707611083984</c:v>
+                  <c:v>2.544198513031006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.459761619567871</c:v>
+                  <c:v>2.516841650009155</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.34212064743042</c:v>
+                  <c:v>1.997059106826782</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.106839179992676</c:v>
+                  <c:v>1.945764780044556</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.031976938247681</c:v>
+                  <c:v>1.730328679084778</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.882252335548401</c:v>
+                  <c:v>1.64141845703125</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.775306105613709</c:v>
+                  <c:v>1.620900750160217</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.700443863868713</c:v>
+                  <c:v>1.61406147480011</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.625581502914429</c:v>
+                  <c:v>1.573026061058044</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.475856900215149</c:v>
+                  <c:v>1.573026061058044</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.347521543502808</c:v>
+                  <c:v>1.55934751033783</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.326132297515869</c:v>
+                  <c:v>1.395205736160278</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.101545333862305</c:v>
+                  <c:v>1.210546135902405</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.037377715110779</c:v>
+                  <c:v>1.176349878311157</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.9839046001434326</c:v>
+                  <c:v>1.073761224746704</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.8555692434310913</c:v>
+                  <c:v>1.046404242515564</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.8127907514572144</c:v>
+                  <c:v>1.039564967155457</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.8127907514572144</c:v>
+                  <c:v>0.9916903376579285</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.7807069420814514</c:v>
+                  <c:v>0.9027801752090454</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.7272338271141052</c:v>
+                  <c:v>0.8617447018623352</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.716539204120636</c:v>
+                  <c:v>0.8070307374000549</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.6630661487579346</c:v>
+                  <c:v>0.7728345394134522</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.6202876567840576</c:v>
+                  <c:v>0.7249597907066345</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.5026469230651856</c:v>
+                  <c:v>0.7112813591957092</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.4812576770782471</c:v>
+                  <c:v>0.6292104125022888</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.4812576770782471</c:v>
+                  <c:v>0.6155319213867188</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.4705630838871002</c:v>
+                  <c:v>0.581335723400116</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.459868460893631</c:v>
+                  <c:v>0.5608179569244385</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.459868460893631</c:v>
+                  <c:v>0.5197824835777283</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.4491738379001617</c:v>
+                  <c:v>0.5129432678222656</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.4170899987220764</c:v>
+                  <c:v>0.4992647767066956</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.4170899987220764</c:v>
+                  <c:v>0.4582293331623077</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.3957007527351379</c:v>
+                  <c:v>0.4582293331623077</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.3957007527351379</c:v>
+                  <c:v>0.4445508420467377</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.3957007527351379</c:v>
+                  <c:v>0.4445508420467377</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.3850061595439911</c:v>
+                  <c:v>0.4171938598155975</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.3636169135570526</c:v>
+                  <c:v>0.3829976320266724</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.3422276973724365</c:v>
+                  <c:v>0.365899533033371</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.3101438283920288</c:v>
+                  <c:v>0.3556406795978546</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.3101438283920288</c:v>
+                  <c:v>0.3488014340400696</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.2673653960227966</c:v>
+                  <c:v>0.3282836973667145</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.2459761500358582</c:v>
+                  <c:v>0.3214444518089294</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.2352815419435501</c:v>
+                  <c:v>0.3077659606933594</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.2138923108577728</c:v>
+                  <c:v>0.2940874695777893</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.2031976878643036</c:v>
+                  <c:v>0.2667304873466492</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.160419225692749</c:v>
+                  <c:v>0.2667304873466492</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.149724617600441</c:v>
+                  <c:v>0.2530520260334015</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.1390299946069717</c:v>
+                  <c:v>0.2325342744588852</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.1390299946069717</c:v>
+                  <c:v>0.2256950438022614</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.1390299946069717</c:v>
+                  <c:v>0.2256950438022614</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.1390299946069717</c:v>
+                  <c:v>0.2188557982444763</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.1283353865146637</c:v>
+                  <c:v>0.1641418486833572</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.09625153988599777</c:v>
+                  <c:v>0.1573026031255722</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.08555692434310913</c:v>
+                  <c:v>0.1436241120100021</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.07486230880022049</c:v>
+                  <c:v>0.1299456208944321</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.06416769325733185</c:v>
+                  <c:v>0.1162671372294426</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.06416769325733185</c:v>
+                  <c:v>0.1162671372294426</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.05347307771444321</c:v>
+                  <c:v>0.09574940800666809</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.04277846217155457</c:v>
+                  <c:v>0.08891016989946365</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.04277846217155457</c:v>
+                  <c:v>0.08891016989946365</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.03208384662866592</c:v>
+                  <c:v>0.08891016989946365</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.03208384662866592</c:v>
+                  <c:v>0.06155319139361382</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.03208384662866592</c:v>
+                  <c:v>0.05471394956111908</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.03208384662866592</c:v>
+                  <c:v>0.04787470400333405</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.02138923108577728</c:v>
+                  <c:v>0.04103546217083931</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.01069461554288864</c:v>
+                  <c:v>0.04103546217083931</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.01069461554288864</c:v>
+                  <c:v>0.03419621661305428</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.01069461554288864</c:v>
+                  <c:v>0.02735697478055954</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.01069461554288864</c:v>
+                  <c:v>0.02735697478055954</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.01069461554288864</c:v>
+                  <c:v>0.02051773108541966</c:v>
                 </c:pt>
                 <c:pt idx="78">
+                  <c:v>0.02051773108541966</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.02051773108541966</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.02051773108541966</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.01367848739027977</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.006839243695139885</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.006839243695139885</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.006839243695139885</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.006839243695139885</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.006839243695139885</c:v>
+                </c:pt>
+                <c:pt idx="87">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1138,8 +1225,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H81" totalsRowCount="1">
-  <autoFilter ref="A2:H80"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H90" totalsRowCount="1">
+  <autoFilter ref="A2:H89"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="ram_percent" totalsRowFunction="sum"/>
@@ -1155,8 +1242,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H81" totalsRowCount="1">
-  <autoFilter ref="A2:H80"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H90" totalsRowCount="1">
+  <autoFilter ref="A2:H89"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="flash_percent" totalsRowFunction="sum"/>
@@ -1456,7 +1543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1472,28 +1559,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1501,25 +1588,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>32.14734268188477</v>
+        <v>40.11637496948242</v>
       </c>
       <c r="C3" s="1">
-        <v>1536</v>
+        <v>2413</v>
       </c>
       <c r="D3" s="1">
-        <v>460</v>
+        <v>569</v>
       </c>
       <c r="E3" s="1">
-        <v>64</v>
+        <v>536</v>
       </c>
       <c r="F3" s="1">
-        <v>396</v>
+        <v>33</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
       <c r="H3" s="1">
-        <v>1536</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1527,25 +1614,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>25.30347442626953</v>
+        <v>25.53615951538086</v>
       </c>
       <c r="C4" s="1">
-        <v>1209</v>
+        <v>1536</v>
       </c>
       <c r="D4" s="1">
-        <v>438</v>
+        <v>460</v>
       </c>
       <c r="E4" s="1">
-        <v>438</v>
+        <v>64</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>396</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>1209</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1553,19 +1640,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>18.16659736633301</v>
+        <v>14.43059062957764</v>
       </c>
       <c r="C5" s="1">
         <v>868</v>
       </c>
       <c r="D5" s="1">
-        <v>160</v>
+        <v>306</v>
       </c>
       <c r="E5" s="1">
-        <v>160</v>
+        <v>286</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -1579,19 +1666,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>11.80410194396973</v>
+        <v>9.376558303833008</v>
       </c>
       <c r="C6" s="1">
         <v>564</v>
       </c>
       <c r="D6" s="1">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="E6" s="1">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -1605,16 +1692,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>3.599832534790039</v>
+        <v>2.859517812728882</v>
       </c>
       <c r="C7" s="1">
         <v>172</v>
       </c>
       <c r="D7" s="1">
-        <v>58</v>
+        <v>130</v>
       </c>
       <c r="E7" s="1">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -1631,7 +1718,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>2.009208917617798</v>
+        <v>1.596009969711304</v>
       </c>
       <c r="C8" s="1">
         <v>96</v>
@@ -1657,7 +1744,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>2.009208917617798</v>
+        <v>1.596009969711304</v>
       </c>
       <c r="C9" s="1">
         <v>96</v>
@@ -1683,16 +1770,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>1.758057713508606</v>
+        <v>1.396508693695068</v>
       </c>
       <c r="C10" s="1">
         <v>84</v>
       </c>
       <c r="D10" s="1">
-        <v>304</v>
+        <v>354</v>
       </c>
       <c r="E10" s="1">
-        <v>304</v>
+        <v>354</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1709,16 +1796,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>1.172038555145264</v>
+        <v>0.9310058355331421</v>
       </c>
       <c r="C11" s="1">
         <v>56</v>
       </c>
       <c r="D11" s="1">
-        <v>206</v>
+        <v>236</v>
       </c>
       <c r="E11" s="1">
-        <v>206</v>
+        <v>236</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1735,16 +1822,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>1.088321447372437</v>
+        <v>0.864505410194397</v>
       </c>
       <c r="C12" s="1">
         <v>52</v>
       </c>
       <c r="D12" s="1">
-        <v>46</v>
+        <v>134</v>
       </c>
       <c r="E12" s="1">
-        <v>46</v>
+        <v>134</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1761,25 +1848,25 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>0.3557974100112915</v>
+        <v>0.5985037684440613</v>
       </c>
       <c r="C13" s="1">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1">
-        <v>893</v>
+        <v>66</v>
       </c>
       <c r="E13" s="1">
-        <v>892</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1787,25 +1874,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>0.1674340665340424</v>
+        <v>0.2327514588832855</v>
       </c>
       <c r="C14" s="1">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1">
-        <v>74</v>
+        <v>1329</v>
       </c>
       <c r="E14" s="1">
-        <v>66</v>
+        <v>1328</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1813,16 +1900,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>0.1674340665340424</v>
+        <v>0.133000835776329</v>
       </c>
       <c r="C15" s="1">
         <v>8</v>
       </c>
       <c r="D15" s="1">
-        <v>1024</v>
+        <v>1598</v>
       </c>
       <c r="E15" s="1">
-        <v>1024</v>
+        <v>1598</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -1839,16 +1926,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>0.08371703326702118</v>
+        <v>0.133000835776329</v>
       </c>
       <c r="C16" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1">
-        <v>856</v>
+        <v>130</v>
       </c>
       <c r="E16" s="1">
-        <v>856</v>
+        <v>130</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -1857,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1865,25 +1952,25 @@
         <v>15</v>
       </c>
       <c r="B17" s="2">
-        <v>0.08371703326702118</v>
+        <v>0.06650041788816452</v>
       </c>
       <c r="C17" s="1">
         <v>4</v>
       </c>
       <c r="D17" s="1">
-        <v>86</v>
+        <v>736</v>
       </c>
       <c r="E17" s="1">
-        <v>18</v>
+        <v>736</v>
       </c>
       <c r="F17" s="1">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
         <v>4</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1891,7 +1978,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2">
-        <v>0.08371703326702118</v>
+        <v>0.06650041788816452</v>
       </c>
       <c r="C18" s="1">
         <v>4</v>
@@ -1900,47 +1987,73 @@
         <v>86</v>
       </c>
       <c r="E18" s="1">
+        <v>18</v>
+      </c>
+      <c r="F18" s="1">
+        <v>64</v>
+      </c>
+      <c r="G18" s="1">
+        <v>4</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.06650041788816452</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1">
+        <v>90</v>
+      </c>
+      <c r="E19" s="1">
         <v>86</v>
       </c>
-      <c r="F18" s="1">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="81" spans="1:8">
-      <c r="A81" t="s">
-        <v>80</v>
-      </c>
-      <c r="B81">
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90">
         <f>SUBTOTAL(109,[ram_percent])</f>
         <v>0</v>
       </c>
-      <c r="C81">
+      <c r="C90">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="D81">
+      <c r="D90">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="E81">
+      <c r="E90">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F81">
+      <c r="F90">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G81">
+      <c r="G90">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H81">
+      <c r="H90">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>
@@ -1956,7 +2069,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1972,45 +2085,45 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2">
-        <v>15.27191066741943</v>
+        <v>13.3843994140625</v>
       </c>
       <c r="C3" s="1">
-        <v>2856</v>
+        <v>3914</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>2856</v>
+        <v>3914</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -2024,19 +2137,19 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2">
-        <v>11.76407718658447</v>
+        <v>10.93595027923584</v>
       </c>
       <c r="C4" s="1">
-        <v>2200</v>
+        <v>3198</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>2200</v>
+        <v>3198</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -2050,19 +2163,19 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2">
-        <v>7.144002914428711</v>
+        <v>7.017064094543457</v>
       </c>
       <c r="C5" s="1">
-        <v>1336</v>
+        <v>2052</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>1336</v>
+        <v>2052</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -2076,19 +2189,19 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2">
-        <v>5.475643157958984</v>
+        <v>6.032212734222412</v>
       </c>
       <c r="C6" s="1">
-        <v>1024</v>
+        <v>1764</v>
       </c>
       <c r="D6" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>1024</v>
+        <v>1764</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -2097,24 +2210,24 @@
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
-        <v>5.208277702331543</v>
+        <v>5.464555740356445</v>
       </c>
       <c r="C7" s="1">
-        <v>974</v>
+        <v>1598</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1">
-        <v>974</v>
+        <v>1598</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -2123,24 +2236,24 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
-        <v>4.775145530700684</v>
+        <v>4.544677257537842</v>
       </c>
       <c r="C8" s="1">
-        <v>893</v>
+        <v>1329</v>
       </c>
       <c r="D8" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1">
-        <v>892</v>
+        <v>1328</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -2149,24 +2262,24 @@
         <v>1</v>
       </c>
       <c r="H8" s="1">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2">
-        <v>4.577295303344727</v>
+        <v>4.363437175750732</v>
       </c>
       <c r="C9" s="1">
-        <v>856</v>
+        <v>1276</v>
       </c>
       <c r="D9" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>856</v>
+        <v>1276</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -2175,24 +2288,24 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2">
-        <v>4.106732368469238</v>
+        <v>3.036624193191528</v>
       </c>
       <c r="C10" s="1">
-        <v>768</v>
+        <v>888</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>768</v>
+        <v>888</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -2206,19 +2319,19 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2">
-        <v>2.566707611083984</v>
+        <v>2.544198513031006</v>
       </c>
       <c r="C11" s="1">
-        <v>480</v>
+        <v>744</v>
       </c>
       <c r="D11" s="1">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>480</v>
+        <v>744</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -2227,50 +2340,50 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2">
-        <v>2.459761619567871</v>
+        <v>2.516841650009155</v>
       </c>
       <c r="C12" s="1">
-        <v>460</v>
+        <v>736</v>
       </c>
       <c r="D12" s="1">
-        <v>1536</v>
+        <v>4</v>
       </c>
       <c r="E12" s="1">
-        <v>64</v>
+        <v>736</v>
       </c>
       <c r="F12" s="1">
-        <v>396</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>1536</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2">
-        <v>2.34212064743042</v>
+        <v>1.997059106826782</v>
       </c>
       <c r="C13" s="1">
-        <v>438</v>
+        <v>584</v>
       </c>
       <c r="D13" s="1">
-        <v>1209</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>438</v>
+        <v>584</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -2279,50 +2392,50 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>1209</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B14" s="2">
-        <v>2.106839179992676</v>
+        <v>1.945764780044556</v>
       </c>
       <c r="C14" s="1">
-        <v>394</v>
+        <v>569</v>
       </c>
       <c r="D14" s="1">
-        <v>0</v>
+        <v>2413</v>
       </c>
       <c r="E14" s="1">
-        <v>394</v>
+        <v>536</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <v>0</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2">
-        <v>2.031976938247681</v>
+        <v>1.730328679084778</v>
       </c>
       <c r="C15" s="1">
-        <v>380</v>
+        <v>506</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>380</v>
+        <v>506</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -2336,19 +2449,19 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2">
-        <v>1.882252335548401</v>
+        <v>1.64141845703125</v>
       </c>
       <c r="C16" s="1">
-        <v>352</v>
+        <v>480</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="E16" s="1">
-        <v>352</v>
+        <v>480</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -2357,24 +2470,24 @@
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2">
-        <v>1.775306105613709</v>
+        <v>1.620900750160217</v>
       </c>
       <c r="C17" s="1">
-        <v>332</v>
+        <v>474</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>332</v>
+        <v>474</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -2388,19 +2501,19 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2">
-        <v>1.700443863868713</v>
+        <v>1.61406147480011</v>
       </c>
       <c r="C18" s="1">
-        <v>318</v>
+        <v>472</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>318</v>
+        <v>472</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
@@ -2414,19 +2527,19 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2">
-        <v>1.625581502914429</v>
+        <v>1.573026061058044</v>
       </c>
       <c r="C19" s="1">
-        <v>304</v>
+        <v>460</v>
       </c>
       <c r="D19" s="1">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>304</v>
+        <v>460</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -2435,50 +2548,50 @@
         <v>0</v>
       </c>
       <c r="H19" s="1">
-        <v>84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B20" s="2">
-        <v>1.475856900215149</v>
+        <v>1.573026061058044</v>
       </c>
       <c r="C20" s="1">
-        <v>276</v>
+        <v>460</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>1536</v>
       </c>
       <c r="E20" s="1">
-        <v>276</v>
+        <v>64</v>
       </c>
       <c r="F20" s="1">
-        <v>0</v>
+        <v>396</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
       </c>
       <c r="H20" s="1">
-        <v>0</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2">
-        <v>1.347521543502808</v>
+        <v>1.55934751033783</v>
       </c>
       <c r="C21" s="1">
-        <v>252</v>
+        <v>456</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>252</v>
+        <v>456</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -2492,19 +2605,19 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2">
-        <v>1.326132297515869</v>
+        <v>1.395205736160278</v>
       </c>
       <c r="C22" s="1">
-        <v>248</v>
+        <v>408</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>248</v>
+        <v>408</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -2518,19 +2631,19 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="2">
-        <v>1.101545333862305</v>
+        <v>1.210546135902405</v>
       </c>
       <c r="C23" s="1">
-        <v>206</v>
+        <v>354</v>
       </c>
       <c r="D23" s="1">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="E23" s="1">
-        <v>206</v>
+        <v>354</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -2539,24 +2652,24 @@
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>56</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2">
-        <v>1.037377715110779</v>
+        <v>1.176349878311157</v>
       </c>
       <c r="C24" s="1">
-        <v>194</v>
+        <v>344</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>194</v>
+        <v>344</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -2570,19 +2683,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2">
-        <v>0.9839046001434326</v>
+        <v>1.073761224746704</v>
       </c>
       <c r="C25" s="1">
-        <v>184</v>
+        <v>314</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>184</v>
+        <v>314</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -2599,19 +2712,19 @@
         <v>3</v>
       </c>
       <c r="B26" s="2">
-        <v>0.8555692434310913</v>
+        <v>1.046404242515564</v>
       </c>
       <c r="C26" s="1">
-        <v>160</v>
+        <v>306</v>
       </c>
       <c r="D26" s="1">
         <v>868</v>
       </c>
       <c r="E26" s="1">
-        <v>160</v>
+        <v>286</v>
       </c>
       <c r="F26" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G26" s="1">
         <v>0</v>
@@ -2622,19 +2735,19 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B27" s="2">
-        <v>0.8127907514572144</v>
+        <v>1.039564967155457</v>
       </c>
       <c r="C27" s="1">
-        <v>152</v>
+        <v>304</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>152</v>
+        <v>304</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -2648,19 +2761,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B28" s="2">
-        <v>0.8127907514572144</v>
+        <v>0.9916903376579285</v>
       </c>
       <c r="C28" s="1">
-        <v>152</v>
+        <v>290</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>152</v>
+        <v>290</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -2674,19 +2787,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B29" s="2">
-        <v>0.7807069420814514</v>
+        <v>0.9027801752090454</v>
       </c>
       <c r="C29" s="1">
-        <v>146</v>
+        <v>264</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>146</v>
+        <v>264</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -2700,19 +2813,19 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B30" s="2">
-        <v>0.7272338271141052</v>
+        <v>0.8617447018623352</v>
       </c>
       <c r="C30" s="1">
-        <v>136</v>
+        <v>252</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>136</v>
+        <v>252</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -2726,19 +2839,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="B31" s="2">
-        <v>0.716539204120636</v>
+        <v>0.8070307374000549</v>
       </c>
       <c r="C31" s="1">
-        <v>134</v>
+        <v>236</v>
       </c>
       <c r="D31" s="1">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="E31" s="1">
-        <v>134</v>
+        <v>236</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -2747,24 +2860,24 @@
         <v>0</v>
       </c>
       <c r="H31" s="1">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B32" s="2">
-        <v>0.6630661487579346</v>
+        <v>0.7728345394134522</v>
       </c>
       <c r="C32" s="1">
-        <v>124</v>
+        <v>226</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>124</v>
+        <v>226</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -2778,19 +2891,19 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B33" s="2">
-        <v>0.6202876567840576</v>
+        <v>0.7249597907066345</v>
       </c>
       <c r="C33" s="1">
-        <v>116</v>
+        <v>212</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>116</v>
+        <v>212</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
@@ -2804,19 +2917,19 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B34" s="2">
-        <v>0.5026469230651856</v>
+        <v>0.7112813591957092</v>
       </c>
       <c r="C34" s="1">
-        <v>94</v>
+        <v>208</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
       </c>
       <c r="E34" s="1">
-        <v>94</v>
+        <v>208</v>
       </c>
       <c r="F34" s="1">
         <v>0</v>
@@ -2830,19 +2943,19 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B35" s="2">
-        <v>0.4812576770782471</v>
+        <v>0.6292104125022888</v>
       </c>
       <c r="C35" s="1">
-        <v>90</v>
+        <v>184</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>90</v>
+        <v>184</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
@@ -2856,19 +2969,19 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B36" s="2">
-        <v>0.4812576770782471</v>
+        <v>0.6155319213867188</v>
       </c>
       <c r="C36" s="1">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
@@ -2882,19 +2995,19 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B37" s="2">
-        <v>0.4705630838871002</v>
+        <v>0.581335723400116</v>
       </c>
       <c r="C37" s="1">
-        <v>88</v>
+        <v>170</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>88</v>
+        <v>170</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -2908,25 +3021,25 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B38" s="2">
-        <v>0.459868460893631</v>
+        <v>0.5608179569244385</v>
       </c>
       <c r="C38" s="1">
-        <v>86</v>
+        <v>164</v>
       </c>
       <c r="D38" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="F38" s="1">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="G38" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H38" s="1">
         <v>0</v>
@@ -2934,19 +3047,19 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B39" s="2">
-        <v>0.459868460893631</v>
+        <v>0.5197824835777283</v>
       </c>
       <c r="C39" s="1">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="D39" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="F39" s="1">
         <v>0</v>
@@ -2955,24 +3068,24 @@
         <v>0</v>
       </c>
       <c r="H39" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B40" s="2">
-        <v>0.4491738379001617</v>
+        <v>0.5129432678222656</v>
       </c>
       <c r="C40" s="1">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="D40" s="1">
-        <v>564</v>
+        <v>0</v>
       </c>
       <c r="E40" s="1">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
@@ -2981,24 +3094,24 @@
         <v>0</v>
       </c>
       <c r="H40" s="1">
-        <v>564</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B41" s="2">
-        <v>0.4170899987220764</v>
+        <v>0.4992647767066956</v>
       </c>
       <c r="C41" s="1">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
@@ -3012,19 +3125,19 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B42" s="2">
-        <v>0.4170899987220764</v>
+        <v>0.4582293331623077</v>
       </c>
       <c r="C42" s="1">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="F42" s="1">
         <v>0</v>
@@ -3038,19 +3151,19 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="B43" s="2">
-        <v>0.3957007527351379</v>
+        <v>0.4582293331623077</v>
       </c>
       <c r="C43" s="1">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="D43" s="1">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E43" s="1">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="F43" s="1">
         <v>0</v>
@@ -3059,76 +3172,76 @@
         <v>0</v>
       </c>
       <c r="H43" s="1">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="B44" s="2">
-        <v>0.3957007527351379</v>
+        <v>0.4445508420467377</v>
       </c>
       <c r="C44" s="1">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="D44" s="1">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="E44" s="1">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="F44" s="1">
         <v>0</v>
       </c>
       <c r="G44" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H44" s="1">
-        <v>0</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B45" s="2">
-        <v>0.3957007527351379</v>
+        <v>0.4445508420467377</v>
       </c>
       <c r="C45" s="1">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="D45" s="1">
         <v>8</v>
       </c>
       <c r="E45" s="1">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="F45" s="1">
         <v>0</v>
       </c>
       <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
         <v>8</v>
-      </c>
-      <c r="H45" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B46" s="2">
-        <v>0.3850061595439911</v>
+        <v>0.4171938598155975</v>
       </c>
       <c r="C46" s="1">
-        <v>72</v>
+        <v>122</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
       </c>
       <c r="E46" s="1">
-        <v>72</v>
+        <v>122</v>
       </c>
       <c r="F46" s="1">
         <v>0</v>
@@ -3142,19 +3255,19 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B47" s="2">
-        <v>0.3636169135570526</v>
+        <v>0.3829976320266724</v>
       </c>
       <c r="C47" s="1">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="D47" s="1">
         <v>0</v>
       </c>
       <c r="E47" s="1">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="F47" s="1">
         <v>0</v>
@@ -3168,45 +3281,45 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="B48" s="2">
-        <v>0.3422276973724365</v>
+        <v>0.365899533033371</v>
       </c>
       <c r="C48" s="1">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="D48" s="1">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="E48" s="1">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="F48" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G48" s="1">
         <v>0</v>
       </c>
       <c r="H48" s="1">
-        <v>0</v>
+        <v>564</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B49" s="2">
-        <v>0.3101438283920288</v>
+        <v>0.3556406795978546</v>
       </c>
       <c r="C49" s="1">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
       </c>
       <c r="E49" s="1">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="F49" s="1">
         <v>0</v>
@@ -3220,45 +3333,45 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B50" s="2">
-        <v>0.3101438283920288</v>
+        <v>0.3488014340400696</v>
       </c>
       <c r="C50" s="1">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="D50" s="1">
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="E50" s="1">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="F50" s="1">
         <v>0</v>
       </c>
       <c r="G50" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H50" s="1">
-        <v>168</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B51" s="2">
-        <v>0.2673653960227966</v>
+        <v>0.3282836973667145</v>
       </c>
       <c r="C51" s="1">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
       </c>
       <c r="E51" s="1">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
@@ -3272,19 +3385,19 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="B52" s="2">
-        <v>0.2459761500358582</v>
+        <v>0.3214444518089294</v>
       </c>
       <c r="C52" s="1">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="D52" s="1">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E52" s="1">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="F52" s="1">
         <v>0</v>
@@ -3293,30 +3406,30 @@
         <v>0</v>
       </c>
       <c r="H52" s="1">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B53" s="2">
-        <v>0.2352815419435501</v>
+        <v>0.3077659606933594</v>
       </c>
       <c r="C53" s="1">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="D53" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E53" s="1">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="F53" s="1">
         <v>0</v>
       </c>
       <c r="G53" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H53" s="1">
         <v>0</v>
@@ -3324,25 +3437,25 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B54" s="2">
-        <v>0.2138923108577728</v>
+        <v>0.2940874695777893</v>
       </c>
       <c r="C54" s="1">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="D54" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E54" s="1">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="F54" s="1">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="G54" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H54" s="1">
         <v>0</v>
@@ -3350,19 +3463,19 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" s="2">
-        <v>0.2031976878643036</v>
+        <v>0.2667304873466492</v>
       </c>
       <c r="C55" s="1">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
       </c>
       <c r="E55" s="1">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="F55" s="1">
         <v>0</v>
@@ -3376,19 +3489,19 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" s="2">
-        <v>0.160419225692749</v>
+        <v>0.2667304873466492</v>
       </c>
       <c r="C56" s="1">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
       </c>
       <c r="E56" s="1">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
@@ -3402,19 +3515,19 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" s="2">
-        <v>0.149724617600441</v>
+        <v>0.2530520260334015</v>
       </c>
       <c r="C57" s="1">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
       </c>
       <c r="E57" s="1">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
@@ -3428,19 +3541,19 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" s="2">
-        <v>0.1390299946069717</v>
+        <v>0.2325342744588852</v>
       </c>
       <c r="C58" s="1">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D58" s="1">
         <v>0</v>
       </c>
       <c r="E58" s="1">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="F58" s="1">
         <v>0</v>
@@ -3454,19 +3567,19 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" s="2">
-        <v>0.1390299946069717</v>
+        <v>0.2256950438022614</v>
       </c>
       <c r="C59" s="1">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
       </c>
       <c r="E59" s="1">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="F59" s="1">
         <v>0</v>
@@ -3480,28 +3593,28 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="B60" s="2">
-        <v>0.1390299946069717</v>
+        <v>0.2256950438022614</v>
       </c>
       <c r="C60" s="1">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="D60" s="1">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E60" s="1">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="F60" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G60" s="1">
         <v>0</v>
       </c>
       <c r="H60" s="1">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -3509,16 +3622,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="2">
-        <v>0.1390299946069717</v>
+        <v>0.2188557982444763</v>
       </c>
       <c r="C61" s="1">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="D61" s="1">
         <v>0</v>
       </c>
       <c r="E61" s="1">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="F61" s="1">
         <v>0</v>
@@ -3535,16 +3648,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="2">
-        <v>0.1283353865146637</v>
+        <v>0.1641418486833572</v>
       </c>
       <c r="C62" s="1">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D62" s="1">
         <v>0</v>
       </c>
       <c r="E62" s="1">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="F62" s="1">
         <v>0</v>
@@ -3561,16 +3674,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="2">
-        <v>0.09625153988599777</v>
+        <v>0.1573026031255722</v>
       </c>
       <c r="C63" s="1">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D63" s="1">
         <v>0</v>
       </c>
       <c r="E63" s="1">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F63" s="1">
         <v>0</v>
@@ -3587,16 +3700,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="2">
-        <v>0.08555692434310913</v>
+        <v>0.1436241120100021</v>
       </c>
       <c r="C64" s="1">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D64" s="1">
         <v>0</v>
       </c>
       <c r="E64" s="1">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F64" s="1">
         <v>0</v>
@@ -3613,16 +3726,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="2">
-        <v>0.07486230880022049</v>
+        <v>0.1299456208944321</v>
       </c>
       <c r="C65" s="1">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D65" s="1">
         <v>0</v>
       </c>
       <c r="E65" s="1">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="F65" s="1">
         <v>0</v>
@@ -3639,16 +3752,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="2">
-        <v>0.06416769325733185</v>
+        <v>0.1162671372294426</v>
       </c>
       <c r="C66" s="1">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D66" s="1">
         <v>0</v>
       </c>
       <c r="E66" s="1">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F66" s="1">
         <v>0</v>
@@ -3665,16 +3778,16 @@
         <v>66</v>
       </c>
       <c r="B67" s="2">
-        <v>0.06416769325733185</v>
+        <v>0.1162671372294426</v>
       </c>
       <c r="C67" s="1">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D67" s="1">
         <v>0</v>
       </c>
       <c r="E67" s="1">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F67" s="1">
         <v>0</v>
@@ -3691,16 +3804,16 @@
         <v>67</v>
       </c>
       <c r="B68" s="2">
-        <v>0.05347307771444321</v>
+        <v>0.09574940800666809</v>
       </c>
       <c r="C68" s="1">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D68" s="1">
         <v>0</v>
       </c>
       <c r="E68" s="1">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F68" s="1">
         <v>0</v>
@@ -3714,19 +3827,19 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="B69" s="2">
-        <v>0.04277846217155457</v>
+        <v>0.08891016989946365</v>
       </c>
       <c r="C69" s="1">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D69" s="1">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="E69" s="1">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F69" s="1">
         <v>0</v>
@@ -3735,24 +3848,24 @@
         <v>0</v>
       </c>
       <c r="H69" s="1">
-        <v>96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B70" s="2">
-        <v>0.04277846217155457</v>
+        <v>0.08891016989946365</v>
       </c>
       <c r="C70" s="1">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D70" s="1">
         <v>0</v>
       </c>
       <c r="E70" s="1">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F70" s="1">
         <v>0</v>
@@ -3766,19 +3879,19 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B71" s="2">
-        <v>0.03208384662866592</v>
+        <v>0.08891016989946365</v>
       </c>
       <c r="C71" s="1">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D71" s="1">
         <v>0</v>
       </c>
       <c r="E71" s="1">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F71" s="1">
         <v>0</v>
@@ -3792,19 +3905,19 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B72" s="2">
-        <v>0.03208384662866592</v>
+        <v>0.06155319139361382</v>
       </c>
       <c r="C72" s="1">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D72" s="1">
         <v>0</v>
       </c>
       <c r="E72" s="1">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F72" s="1">
         <v>0</v>
@@ -3818,19 +3931,19 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B73" s="2">
-        <v>0.03208384662866592</v>
+        <v>0.05471394956111908</v>
       </c>
       <c r="C73" s="1">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
       </c>
       <c r="E73" s="1">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F73" s="1">
         <v>0</v>
@@ -3844,19 +3957,19 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B74" s="2">
-        <v>0.03208384662866592</v>
+        <v>0.04787470400333405</v>
       </c>
       <c r="C74" s="1">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D74" s="1">
         <v>0</v>
       </c>
       <c r="E74" s="1">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F74" s="1">
         <v>0</v>
@@ -3870,22 +3983,22 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B75" s="2">
-        <v>0.02138923108577728</v>
+        <v>0.04103546217083931</v>
       </c>
       <c r="C75" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D75" s="1">
         <v>0</v>
       </c>
       <c r="E75" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F75" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G75" s="1">
         <v>0</v>
@@ -3896,19 +4009,19 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B76" s="2">
-        <v>0.01069461554288864</v>
+        <v>0.04103546217083931</v>
       </c>
       <c r="C76" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D76" s="1">
         <v>0</v>
       </c>
       <c r="E76" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F76" s="1">
         <v>0</v>
@@ -3922,19 +4035,19 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B77" s="2">
-        <v>0.01069461554288864</v>
+        <v>0.03419621661305428</v>
       </c>
       <c r="C77" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D77" s="1">
         <v>0</v>
       </c>
       <c r="E77" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F77" s="1">
         <v>0</v>
@@ -3948,19 +4061,19 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="1" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B78" s="2">
-        <v>0.01069461554288864</v>
+        <v>0.02735697478055954</v>
       </c>
       <c r="C78" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D78" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="E78" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F78" s="1">
         <v>0</v>
@@ -3969,7 +4082,7 @@
         <v>0</v>
       </c>
       <c r="H78" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3977,16 +4090,16 @@
         <v>77</v>
       </c>
       <c r="B79" s="2">
-        <v>0.01069461554288864</v>
+        <v>0.02735697478055954</v>
       </c>
       <c r="C79" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D79" s="1">
         <v>0</v>
       </c>
       <c r="E79" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F79" s="1">
         <v>0</v>
@@ -4003,56 +4116,290 @@
         <v>78</v>
       </c>
       <c r="B80" s="2">
-        <v>0.01069461554288864</v>
+        <v>0.02051773108541966</v>
       </c>
       <c r="C80" s="1">
+        <v>6</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0</v>
+      </c>
+      <c r="E80" s="1">
+        <v>6</v>
+      </c>
+      <c r="F80" s="1">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1">
+        <v>0</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81" s="2">
+        <v>0.02051773108541966</v>
+      </c>
+      <c r="C81" s="1">
+        <v>6</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0</v>
+      </c>
+      <c r="E81" s="1">
+        <v>6</v>
+      </c>
+      <c r="F81" s="1">
+        <v>0</v>
+      </c>
+      <c r="G81" s="1">
+        <v>0</v>
+      </c>
+      <c r="H81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B82" s="2">
+        <v>0.02051773108541966</v>
+      </c>
+      <c r="C82" s="1">
+        <v>6</v>
+      </c>
+      <c r="D82" s="1">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1">
+        <v>6</v>
+      </c>
+      <c r="F82" s="1">
+        <v>0</v>
+      </c>
+      <c r="G82" s="1">
+        <v>0</v>
+      </c>
+      <c r="H82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="2">
+        <v>0.02051773108541966</v>
+      </c>
+      <c r="C83" s="1">
+        <v>6</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1">
+        <v>6</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1">
+        <v>0</v>
+      </c>
+      <c r="H83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" s="2">
+        <v>0.01367848739027977</v>
+      </c>
+      <c r="C84" s="1">
+        <v>4</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0</v>
+      </c>
+      <c r="F84" s="1">
+        <v>4</v>
+      </c>
+      <c r="G84" s="1">
+        <v>0</v>
+      </c>
+      <c r="H84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" s="2">
+        <v>0.006839243695139885</v>
+      </c>
+      <c r="C85" s="1">
         <v>2</v>
       </c>
-      <c r="D80" s="1">
-        <v>0</v>
-      </c>
-      <c r="E80" s="1">
+      <c r="D85" s="1">
+        <v>0</v>
+      </c>
+      <c r="E85" s="1">
         <v>2</v>
       </c>
-      <c r="F80" s="1">
-        <v>0</v>
-      </c>
-      <c r="G80" s="1">
-        <v>0</v>
-      </c>
-      <c r="H80" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
-      <c r="A81" t="s">
-        <v>80</v>
-      </c>
-      <c r="B81">
+      <c r="F85" s="1">
+        <v>0</v>
+      </c>
+      <c r="G85" s="1">
+        <v>0</v>
+      </c>
+      <c r="H85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B86" s="2">
+        <v>0.006839243695139885</v>
+      </c>
+      <c r="C86" s="1">
+        <v>2</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0</v>
+      </c>
+      <c r="E86" s="1">
+        <v>2</v>
+      </c>
+      <c r="F86" s="1">
+        <v>0</v>
+      </c>
+      <c r="G86" s="1">
+        <v>0</v>
+      </c>
+      <c r="H86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" s="2">
+        <v>0.006839243695139885</v>
+      </c>
+      <c r="C87" s="1">
+        <v>2</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0</v>
+      </c>
+      <c r="E87" s="1">
+        <v>2</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0</v>
+      </c>
+      <c r="G87" s="1">
+        <v>0</v>
+      </c>
+      <c r="H87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88" s="2">
+        <v>0.006839243695139885</v>
+      </c>
+      <c r="C88" s="1">
+        <v>2</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0</v>
+      </c>
+      <c r="E88" s="1">
+        <v>2</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1">
+        <v>0</v>
+      </c>
+      <c r="H88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B89" s="2">
+        <v>0.006839243695139885</v>
+      </c>
+      <c r="C89" s="1">
+        <v>2</v>
+      </c>
+      <c r="D89" s="1">
+        <v>0</v>
+      </c>
+      <c r="E89" s="1">
+        <v>2</v>
+      </c>
+      <c r="F89" s="1">
+        <v>0</v>
+      </c>
+      <c r="G89" s="1">
+        <v>0</v>
+      </c>
+      <c r="H89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90">
         <f>SUBTOTAL(109,[flash_percent])</f>
         <v>0</v>
       </c>
-      <c r="C81">
+      <c r="C90">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="D81">
+      <c r="D90">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="E81">
+      <c r="E90">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F81">
+      <c r="F90">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G81">
+      <c r="G90">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H81">
+      <c r="H90">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>

</xml_diff>